<commit_message>
App organization / Bid Sheet start
</commit_message>
<xml_diff>
--- a/CageCodelist.xlsx
+++ b/CageCodelist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avinash Patel\Desktop\WestSim_App\WestSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66E59B6-24AD-49AB-B308-16EE377B57D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118AD33F-D088-42F6-A03E-EB33C2B1BB7E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1470" windowWidth="29040" windowHeight="15840" firstSheet="16" activeTab="16" xr2:uid="{BFAE7096-C865-48E4-884B-BB11FAFA2759}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="16" activeTab="16" xr2:uid="{BFAE7096-C865-48E4-884B-BB11FAFA2759}"/>
   </bookViews>
   <sheets>
     <sheet name="QuoteCal" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1432,7 +1432,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9479" uniqueCount="5894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9481" uniqueCount="5893">
   <si>
     <t>TSE</t>
   </si>
@@ -19189,10 +19189,7 @@
     <t>samantha.gorney@vteworld.com</t>
   </si>
   <si>
-    <t>34914</t>
-  </si>
-  <si>
-    <t>pg</t>
+    <t>p g</t>
   </si>
   <si>
     <t>g</t>
@@ -19208,7 +19205,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
-  <fonts count="59">
+  <fonts count="61">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -19603,6 +19600,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
@@ -19611,7 +19624,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -19704,11 +19717,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF0F0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -19930,21 +19949,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF3C4B78"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF3C4B78"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF3C4B78"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -19954,7 +19958,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="57" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="57" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -20190,11 +20194,17 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="58" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="16" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="60" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="17" borderId="0" xfId="4"/>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -20212,12 +20222,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -30044,8 +30048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA825E1-D4F3-4B14-9B07-A99A0DC7EB36}">
   <dimension ref="A1:G333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30059,8 +30063,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.15" customHeight="1">
-      <c r="A1" s="199"/>
-      <c r="B1" s="200" t="s">
+      <c r="A1" s="201" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B1" s="202" t="s">
         <v>4405</v>
       </c>
       <c r="C1" t="s">
@@ -30071,8 +30077,8 @@
       <c r="F1" s="83"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="199"/>
-      <c r="B2" s="200" t="s">
+      <c r="A2" s="201"/>
+      <c r="B2" s="202" t="s">
         <v>747</v>
       </c>
       <c r="C2" t="s">
@@ -30085,8 +30091,8 @@
       <c r="F2" s="83"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="199"/>
-      <c r="B3" s="200" t="s">
+      <c r="A3" s="201"/>
+      <c r="B3" s="202" t="s">
         <v>4239</v>
       </c>
       <c r="C3" t="s">
@@ -30099,8 +30105,8 @@
       <c r="F3" s="83"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="199"/>
-      <c r="B4" s="200" t="s">
+      <c r="A4" s="201"/>
+      <c r="B4" s="202" t="s">
         <v>5825</v>
       </c>
       <c r="C4" t="s">
@@ -30111,8 +30117,8 @@
       <c r="F4" s="83"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="199"/>
-      <c r="B5" s="200">
+      <c r="A5" s="201"/>
+      <c r="B5" s="202">
         <v>70508</v>
       </c>
       <c r="C5" t="s">
@@ -30125,8 +30131,8 @@
       <c r="F5" s="83"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="199"/>
-      <c r="B6" s="200" t="s">
+      <c r="A6" s="201"/>
+      <c r="B6" s="202" t="s">
         <v>4346</v>
       </c>
       <c r="C6" t="s">
@@ -30139,8 +30145,8 @@
       <c r="F6" s="83"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="199"/>
-      <c r="B7" s="202">
+      <c r="A7" s="201"/>
+      <c r="B7" s="204">
         <v>91663</v>
       </c>
       <c r="C7" t="s">
@@ -30151,14 +30157,16 @@
       <c r="F7" s="83"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="199"/>
-      <c r="B8" s="200" t="s">
+      <c r="A8" s="201" t="s">
+        <v>5891</v>
+      </c>
+      <c r="B8" s="202" t="s">
         <v>253</v>
       </c>
       <c r="C8" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="205" t="s">
+      <c r="D8" s="207" t="s">
         <v>4243</v>
       </c>
       <c r="E8" s="186" t="s">
@@ -30170,8 +30178,8 @@
       <c r="G8" s="186"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="199"/>
-      <c r="B9" s="200" t="s">
+      <c r="A9" s="201"/>
+      <c r="B9" s="202" t="s">
         <v>1682</v>
       </c>
       <c r="C9" t="s">
@@ -30185,8 +30193,8 @@
       <c r="G9" s="131"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="199"/>
-      <c r="B10" s="200" t="s">
+      <c r="A10" s="201"/>
+      <c r="B10" s="202" t="s">
         <v>4492</v>
       </c>
       <c r="C10" t="s">
@@ -30197,14 +30205,14 @@
       <c r="F10" s="83"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="199"/>
-      <c r="B11" s="200" t="s">
+      <c r="A11" s="201"/>
+      <c r="B11" s="202" t="s">
         <v>4722</v>
       </c>
       <c r="C11" t="s">
         <v>4246</v>
       </c>
-      <c r="D11" s="204" t="s">
+      <c r="D11" s="206" t="s">
         <v>5867</v>
       </c>
       <c r="E11" s="186" t="s">
@@ -30213,8 +30221,8 @@
       <c r="F11" s="186"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="199"/>
-      <c r="B12" s="200" t="s">
+      <c r="A12" s="201"/>
+      <c r="B12" s="202" t="s">
         <v>159</v>
       </c>
       <c r="C12" t="s">
@@ -30225,8 +30233,8 @@
       <c r="F12" s="83"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="199"/>
-      <c r="B13" s="200" t="s">
+      <c r="A13" s="201"/>
+      <c r="B13" s="202" t="s">
         <v>221</v>
       </c>
       <c r="C13" t="s">
@@ -30239,8 +30247,8 @@
       <c r="F13" s="83"/>
     </row>
     <row r="14" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A14" s="199"/>
-      <c r="B14" s="200" t="s">
+      <c r="A14" s="201"/>
+      <c r="B14" s="202" t="s">
         <v>379</v>
       </c>
       <c r="C14" t="s">
@@ -30253,8 +30261,8 @@
       <c r="F14" s="83"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="199"/>
-      <c r="B15" s="200" t="s">
+      <c r="A15" s="201"/>
+      <c r="B15" s="202" t="s">
         <v>150</v>
       </c>
       <c r="C15" t="s">
@@ -30267,8 +30275,8 @@
       <c r="F15" s="83"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="199"/>
-      <c r="B16" s="200" t="s">
+      <c r="A16" s="201"/>
+      <c r="B16" s="202" t="s">
         <v>4376</v>
       </c>
       <c r="C16" t="s">
@@ -30281,22 +30289,22 @@
       <c r="F16" s="83"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A17" s="199"/>
-      <c r="B17" s="200">
+      <c r="A17" s="201"/>
+      <c r="B17" s="202">
         <v>76096</v>
       </c>
       <c r="C17" t="s">
         <v>4403</v>
       </c>
-      <c r="D17" s="204" t="s">
+      <c r="D17" s="206" t="s">
         <v>5868</v>
       </c>
-      <c r="E17" s="198"/>
+      <c r="E17" s="199"/>
       <c r="F17" s="83"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="199"/>
-      <c r="B18" s="202" t="s">
+      <c r="A18" s="201"/>
+      <c r="B18" s="204" t="s">
         <v>466</v>
       </c>
       <c r="C18" t="s">
@@ -30305,12 +30313,12 @@
       <c r="D18" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E18" s="198"/>
+      <c r="E18" s="199"/>
       <c r="F18" s="83"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="199"/>
-      <c r="B19" s="202">
+      <c r="A19" s="201"/>
+      <c r="B19" s="204">
         <v>51435</v>
       </c>
       <c r="C19" t="s">
@@ -30323,8 +30331,8 @@
       <c r="F19" s="83"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="199"/>
-      <c r="B20" s="200" t="s">
+      <c r="A20" s="201"/>
+      <c r="B20" s="202" t="s">
         <v>4332</v>
       </c>
       <c r="C20" t="s">
@@ -30337,8 +30345,8 @@
       <c r="F20" s="83"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="199"/>
-      <c r="B21" s="200" t="s">
+      <c r="A21" s="201"/>
+      <c r="B21" s="202" t="s">
         <v>91</v>
       </c>
       <c r="C21" t="s">
@@ -30349,8 +30357,8 @@
       <c r="F21" s="83"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="199"/>
-      <c r="B22" s="203" t="s">
+      <c r="A22" s="201"/>
+      <c r="B22" s="205" t="s">
         <v>1417</v>
       </c>
       <c r="C22" t="s">
@@ -30363,10 +30371,10 @@
       <c r="F22" s="83"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="199" t="s">
-        <v>5892</v>
-      </c>
-      <c r="B23" s="200" t="s">
+      <c r="A23" s="201" t="s">
+        <v>5891</v>
+      </c>
+      <c r="B23" s="202" t="s">
         <v>110</v>
       </c>
       <c r="C23" t="s">
@@ -30379,8 +30387,8 @@
       <c r="F23" s="83"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="199"/>
-      <c r="B24" s="200" t="s">
+      <c r="A24" s="201"/>
+      <c r="B24" s="202" t="s">
         <v>394</v>
       </c>
       <c r="C24" t="s">
@@ -30393,8 +30401,8 @@
       <c r="F24" s="83"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="199"/>
-      <c r="B25" s="200" t="s">
+      <c r="A25" s="201"/>
+      <c r="B25" s="202" t="s">
         <v>517</v>
       </c>
       <c r="C25" t="s">
@@ -30409,9 +30417,9 @@
       <c r="F25" s="83"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="199"/>
-      <c r="B26" s="200" t="s">
-        <v>5891</v>
+      <c r="A26" s="201"/>
+      <c r="B26" s="202">
+        <v>34914</v>
       </c>
       <c r="C26" t="s">
         <v>4270</v>
@@ -30423,10 +30431,10 @@
       <c r="F26" s="83"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="199" t="s">
-        <v>5893</v>
-      </c>
-      <c r="B27" s="202" t="s">
+      <c r="A27" s="201" t="s">
+        <v>5892</v>
+      </c>
+      <c r="B27" s="204" t="s">
         <v>636</v>
       </c>
       <c r="C27" t="s">
@@ -30435,12 +30443,12 @@
       <c r="D27" s="10" t="s">
         <v>678</v>
       </c>
-      <c r="E27" s="197"/>
+      <c r="E27" s="198"/>
       <c r="F27" s="83"/>
     </row>
     <row r="28" spans="1:6" ht="19.899999999999999" customHeight="1">
-      <c r="A28" s="199"/>
-      <c r="B28" s="200" t="s">
+      <c r="A28" s="201"/>
+      <c r="B28" s="202" t="s">
         <v>4323</v>
       </c>
       <c r="C28" t="s">
@@ -30453,8 +30461,8 @@
       <c r="F28" s="83"/>
     </row>
     <row r="29" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A29" s="199"/>
-      <c r="B29" s="200"/>
+      <c r="A29" s="201"/>
+      <c r="B29" s="202"/>
       <c r="C29" t="s">
         <v>4480</v>
       </c>
@@ -30465,8 +30473,8 @@
       <c r="F29" s="83"/>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
-      <c r="A30" s="199"/>
-      <c r="B30" s="200">
+      <c r="A30" s="201"/>
+      <c r="B30" s="202">
         <v>57715</v>
       </c>
       <c r="C30" t="s">
@@ -30479,8 +30487,8 @@
       <c r="F30" s="83"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="199"/>
-      <c r="B31" s="200" t="s">
+      <c r="A31" s="201"/>
+      <c r="B31" s="202" t="s">
         <v>4353</v>
       </c>
       <c r="C31" t="s">
@@ -30491,8 +30499,8 @@
       <c r="F31" s="83"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="199"/>
-      <c r="B32" s="201" t="s">
+      <c r="A32" s="201"/>
+      <c r="B32" s="203" t="s">
         <v>987</v>
       </c>
       <c r="C32" t="s">
@@ -30505,8 +30513,8 @@
       <c r="F32" s="83"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="199"/>
-      <c r="B33" s="200" t="s">
+      <c r="A33" s="201"/>
+      <c r="B33" s="202" t="s">
         <v>1673</v>
       </c>
       <c r="C33" t="s">
@@ -30519,8 +30527,8 @@
       <c r="F33" s="83"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="199"/>
-      <c r="B34" s="200" t="s">
+      <c r="A34" s="201"/>
+      <c r="B34" s="202" t="s">
         <v>4942</v>
       </c>
       <c r="C34" t="s">
@@ -30531,8 +30539,8 @@
       <c r="F34" s="83"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="199"/>
-      <c r="B35" s="200" t="s">
+      <c r="A35" s="201"/>
+      <c r="B35" s="202" t="s">
         <v>1863</v>
       </c>
       <c r="C35" t="s">
@@ -30543,8 +30551,8 @@
       <c r="F35" s="83"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="199"/>
-      <c r="B36" s="200">
+      <c r="A36" s="201"/>
+      <c r="B36" s="202">
         <v>43321</v>
       </c>
       <c r="C36" t="s">
@@ -30555,8 +30563,8 @@
       <c r="F36" s="83"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="199"/>
-      <c r="B37" s="202" t="s">
+      <c r="A37" s="201"/>
+      <c r="B37" s="204" t="s">
         <v>502</v>
       </c>
       <c r="C37" t="s">
@@ -30569,8 +30577,8 @@
       <c r="F37" s="83"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="199"/>
-      <c r="B38" s="202" t="s">
+      <c r="A38" s="201"/>
+      <c r="B38" s="204" t="s">
         <v>4474</v>
       </c>
       <c r="C38" t="s">
@@ -30581,8 +30589,8 @@
       <c r="F38" s="83"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="199"/>
-      <c r="B39" s="200" t="s">
+      <c r="A39" s="201"/>
+      <c r="B39" s="202" t="s">
         <v>1166</v>
       </c>
       <c r="C39" t="s">
@@ -30595,8 +30603,8 @@
       <c r="F39" s="83"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="199"/>
-      <c r="B40" s="200">
+      <c r="A40" s="201"/>
+      <c r="B40" s="202">
         <v>87009</v>
       </c>
       <c r="C40" t="s">
@@ -30609,8 +30617,8 @@
       <c r="F40" s="83"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="199"/>
-      <c r="B41" s="200" t="s">
+      <c r="A41" s="201"/>
+      <c r="B41" s="202" t="s">
         <v>4445</v>
       </c>
       <c r="C41" t="s">
@@ -30621,8 +30629,10 @@
       <c r="F41" s="83"/>
     </row>
     <row r="42" spans="1:6" ht="18" customHeight="1">
-      <c r="A42" s="199"/>
-      <c r="B42" s="200" t="s">
+      <c r="A42" s="201" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B42" s="202" t="s">
         <v>446</v>
       </c>
       <c r="C42" t="s">
@@ -30635,20 +30645,20 @@
       <c r="F42" s="83"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="199"/>
-      <c r="B43" s="200" t="s">
+      <c r="A43" s="201"/>
+      <c r="B43" s="202" t="s">
         <v>449</v>
       </c>
       <c r="C43" t="s">
         <v>448</v>
       </c>
-      <c r="D43" s="197"/>
-      <c r="E43" s="197"/>
+      <c r="D43" s="198"/>
+      <c r="E43" s="198"/>
       <c r="F43" s="83"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="199"/>
-      <c r="B44" s="200" t="s">
+      <c r="A44" s="201"/>
+      <c r="B44" s="202" t="s">
         <v>4278</v>
       </c>
       <c r="C44" t="s">
@@ -30661,8 +30671,8 @@
       <c r="F44" s="83"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="199"/>
-      <c r="B45" s="200" t="s">
+      <c r="A45" s="201"/>
+      <c r="B45" s="202" t="s">
         <v>225</v>
       </c>
       <c r="C45" t="s">
@@ -30675,8 +30685,8 @@
       <c r="F45" s="83"/>
     </row>
     <row r="46" spans="1:6" ht="16.899999999999999" customHeight="1">
-      <c r="A46" s="199"/>
-      <c r="B46" s="200">
+      <c r="A46" s="201"/>
+      <c r="B46" s="202">
         <v>32387</v>
       </c>
       <c r="C46" t="s">
@@ -30689,8 +30699,8 @@
       <c r="F46" s="83"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="199"/>
-      <c r="B47" s="200" t="s">
+      <c r="A47" s="201"/>
+      <c r="B47" s="202" t="s">
         <v>818</v>
       </c>
       <c r="C47" t="s">
@@ -30703,8 +30713,8 @@
       <c r="F47" s="83"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="199"/>
-      <c r="B48" s="200" t="s">
+      <c r="A48" s="201"/>
+      <c r="B48" s="202" t="s">
         <v>456</v>
       </c>
       <c r="C48" t="s">
@@ -30715,8 +30725,8 @@
       <c r="F48" s="83"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="199"/>
-      <c r="B49" s="200" t="s">
+      <c r="A49" s="201"/>
+      <c r="B49" s="202" t="s">
         <v>616</v>
       </c>
       <c r="C49" t="s">
@@ -30729,22 +30739,22 @@
       <c r="F49" s="83"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="199"/>
-      <c r="B50" s="200" t="s">
+      <c r="A50" s="201"/>
+      <c r="B50" s="202" t="s">
         <v>4314</v>
       </c>
       <c r="C50" t="s">
         <v>4315</v>
       </c>
-      <c r="D50" s="204" t="s">
+      <c r="D50" s="206" t="s">
         <v>5874</v>
       </c>
       <c r="E50" s="186"/>
       <c r="F50" s="83"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="199"/>
-      <c r="B51" s="200" t="s">
+      <c r="A51" s="201"/>
+      <c r="B51" s="202" t="s">
         <v>4422</v>
       </c>
       <c r="C51" t="s">
@@ -30757,8 +30767,8 @@
       <c r="F51" s="83"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="199"/>
-      <c r="B52" s="200" t="s">
+      <c r="A52" s="201"/>
+      <c r="B52" s="202" t="s">
         <v>157</v>
       </c>
       <c r="C52" t="s">
@@ -30773,8 +30783,8 @@
       <c r="F52" s="83"/>
     </row>
     <row r="53" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A53" s="199"/>
-      <c r="B53" s="200" t="s">
+      <c r="A53" s="201"/>
+      <c r="B53" s="202" t="s">
         <v>4292</v>
       </c>
       <c r="C53" t="s">
@@ -30787,8 +30797,8 @@
       <c r="F53" s="83"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="199"/>
-      <c r="B54" s="200" t="s">
+      <c r="A54" s="201"/>
+      <c r="B54" s="202" t="s">
         <v>412</v>
       </c>
       <c r="C54" t="s">
@@ -30801,8 +30811,8 @@
       <c r="F54" s="83"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="199"/>
-      <c r="B55" s="200" t="s">
+      <c r="A55" s="201"/>
+      <c r="B55" s="202" t="s">
         <v>534</v>
       </c>
       <c r="C55" t="s">
@@ -30815,8 +30825,8 @@
       <c r="F55" s="83"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="199"/>
-      <c r="B56" s="200" t="s">
+      <c r="A56" s="201"/>
+      <c r="B56" s="202" t="s">
         <v>1329</v>
       </c>
       <c r="C56" t="s">
@@ -30825,12 +30835,12 @@
       <c r="D56" s="10" t="s">
         <v>1331</v>
       </c>
-      <c r="E56" s="198"/>
+      <c r="E56" s="199"/>
       <c r="F56" s="83"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="199"/>
-      <c r="B57" s="200" t="s">
+      <c r="A57" s="201"/>
+      <c r="B57" s="202" t="s">
         <v>437</v>
       </c>
       <c r="C57" t="s">
@@ -30843,8 +30853,8 @@
       <c r="F57" s="83"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="199"/>
-      <c r="B58" s="200">
+      <c r="A58" s="201"/>
+      <c r="B58" s="202">
         <v>82199</v>
       </c>
       <c r="C58" t="s">
@@ -30857,8 +30867,8 @@
       <c r="F58" s="83"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="199"/>
-      <c r="B59" s="200" t="s">
+      <c r="A59" s="201"/>
+      <c r="B59" s="202" t="s">
         <v>4758</v>
       </c>
       <c r="C59" t="s">
@@ -30871,8 +30881,8 @@
       <c r="F59" s="83"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="199"/>
-      <c r="B60" s="202" t="s">
+      <c r="A60" s="201"/>
+      <c r="B60" s="204" t="s">
         <v>4476</v>
       </c>
       <c r="C60" t="s">
@@ -30883,8 +30893,8 @@
       <c r="F60" s="83"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="199"/>
-      <c r="B61" s="200" t="s">
+      <c r="A61" s="201"/>
+      <c r="B61" s="202" t="s">
         <v>4881</v>
       </c>
       <c r="C61" t="s">
@@ -30895,8 +30905,8 @@
       <c r="F61" s="83"/>
     </row>
     <row r="62" spans="1:6" ht="16.899999999999999" customHeight="1" thickBot="1">
-      <c r="A62" s="199"/>
-      <c r="B62" s="200" t="s">
+      <c r="A62" s="201"/>
+      <c r="B62" s="202" t="s">
         <v>4280</v>
       </c>
       <c r="C62" t="s">
@@ -30907,20 +30917,20 @@
       <c r="F62" s="83"/>
     </row>
     <row r="63" spans="1:6" ht="16.899999999999999" customHeight="1" thickBot="1">
-      <c r="A63" s="199"/>
-      <c r="B63" s="202" t="s">
+      <c r="A63" s="201"/>
+      <c r="B63" s="204" t="s">
         <v>283</v>
       </c>
       <c r="C63" t="s">
         <v>520</v>
       </c>
       <c r="D63" s="186"/>
-      <c r="E63" s="207"/>
+      <c r="E63" s="200"/>
       <c r="F63" s="83"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A64" s="199"/>
-      <c r="B64" s="200" t="s">
+      <c r="A64" s="201"/>
+      <c r="B64" s="202" t="s">
         <v>540</v>
       </c>
       <c r="C64" t="s">
@@ -30930,11 +30940,11 @@
         <v>670</v>
       </c>
       <c r="E64" s="186"/>
-      <c r="F64" s="206"/>
+      <c r="F64" s="197"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="199"/>
-      <c r="B65" s="200">
+      <c r="A65" s="201"/>
+      <c r="B65" s="202">
         <v>66647</v>
       </c>
       <c r="C65" t="s">
@@ -30947,8 +30957,8 @@
       <c r="F65" s="83"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="199"/>
-      <c r="B66" s="200">
+      <c r="A66" s="201"/>
+      <c r="B66" s="202">
         <v>50541</v>
       </c>
       <c r="C66" t="s">
@@ -30961,8 +30971,8 @@
       <c r="F66" s="83"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="199"/>
-      <c r="B67" s="200">
+      <c r="A67" s="201"/>
+      <c r="B67" s="202">
         <v>24602</v>
       </c>
       <c r="C67" t="s">
@@ -30975,8 +30985,8 @@
       <c r="F67" s="83"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="199"/>
-      <c r="B68" s="200" t="s">
+      <c r="A68" s="201"/>
+      <c r="B68" s="202" t="s">
         <v>4337</v>
       </c>
       <c r="C68" t="s">
@@ -30989,8 +30999,8 @@
       <c r="F68" s="83"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="199"/>
-      <c r="B69" s="200" t="s">
+      <c r="A69" s="201"/>
+      <c r="B69" s="202" t="s">
         <v>4368</v>
       </c>
       <c r="C69" t="s">
@@ -31003,8 +31013,8 @@
       <c r="F69" s="83"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="199"/>
-      <c r="B70" s="200">
+      <c r="A70" s="201"/>
+      <c r="B70" s="202">
         <v>64411</v>
       </c>
       <c r="C70" t="s">
@@ -31013,14 +31023,14 @@
       <c r="D70" s="10" t="s">
         <v>5879</v>
       </c>
-      <c r="E70" s="197" t="s">
+      <c r="E70" s="198" t="s">
         <v>4370</v>
       </c>
       <c r="F70" s="83"/>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1">
-      <c r="A71" s="199"/>
-      <c r="B71" s="200" t="s">
+      <c r="A71" s="201"/>
+      <c r="B71" s="202" t="s">
         <v>5852</v>
       </c>
       <c r="C71" t="s">
@@ -31031,8 +31041,8 @@
       <c r="F71" s="83"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="199"/>
-      <c r="B72" s="200" t="s">
+      <c r="A72" s="201"/>
+      <c r="B72" s="202" t="s">
         <v>4418</v>
       </c>
       <c r="C72" t="s">
@@ -31041,12 +31051,12 @@
       <c r="D72" s="10" t="s">
         <v>5880</v>
       </c>
-      <c r="E72" s="197"/>
+      <c r="E72" s="198"/>
       <c r="F72" s="83"/>
     </row>
     <row r="73" spans="1:6" ht="17.649999999999999" customHeight="1">
-      <c r="A73" s="199"/>
-      <c r="B73" s="200">
+      <c r="A73" s="201"/>
+      <c r="B73" s="202">
         <v>58860</v>
       </c>
       <c r="C73" t="s">
@@ -31055,14 +31065,14 @@
       <c r="D73" s="10" t="s">
         <v>4478</v>
       </c>
-      <c r="E73" s="198" t="s">
+      <c r="E73" s="199" t="s">
         <v>4420</v>
       </c>
       <c r="F73" s="83"/>
     </row>
     <row r="74" spans="1:6" ht="16.149999999999999" customHeight="1">
-      <c r="A74" s="199"/>
-      <c r="B74" s="200" t="s">
+      <c r="A74" s="201"/>
+      <c r="B74" s="202" t="s">
         <v>1632</v>
       </c>
       <c r="C74" t="s">
@@ -31075,8 +31085,8 @@
       <c r="F74" s="83"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="199"/>
-      <c r="B75" s="200">
+      <c r="A75" s="201"/>
+      <c r="B75" s="202">
         <v>44256</v>
       </c>
       <c r="C75" t="s">
@@ -31089,8 +31099,8 @@
       <c r="F75" s="83"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="199"/>
-      <c r="B76" s="200" t="s">
+      <c r="A76" s="201"/>
+      <c r="B76" s="202" t="s">
         <v>1573</v>
       </c>
       <c r="C76" t="s">
@@ -31103,8 +31113,8 @@
       <c r="F76" s="83"/>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="199"/>
-      <c r="B77" s="200" t="s">
+      <c r="A77" s="201"/>
+      <c r="B77" s="202" t="s">
         <v>4372</v>
       </c>
       <c r="C77" t="s">
@@ -31117,8 +31127,8 @@
       <c r="F77" s="83"/>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="199"/>
-      <c r="B78" s="200" t="s">
+      <c r="A78" s="201"/>
+      <c r="B78" s="202" t="s">
         <v>4765</v>
       </c>
       <c r="C78" t="s">
@@ -31131,8 +31141,8 @@
       <c r="F78" s="83"/>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="199"/>
-      <c r="B79" s="200" t="s">
+      <c r="A79" s="201"/>
+      <c r="B79" s="202" t="s">
         <v>1168</v>
       </c>
       <c r="C79" t="s">
@@ -31146,7 +31156,7 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="83"/>
-      <c r="B80" s="200" t="s">
+      <c r="B80" s="202" t="s">
         <v>4472</v>
       </c>
       <c r="C80" t="s">
@@ -31158,7 +31168,7 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="83"/>
-      <c r="B81" s="200" t="s">
+      <c r="B81" s="202" t="s">
         <v>5855</v>
       </c>
       <c r="C81" t="s">
@@ -31170,7 +31180,7 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="83"/>
-      <c r="B82" s="200">
+      <c r="B82" s="202">
         <v>61141</v>
       </c>
       <c r="C82" t="s">
@@ -31182,7 +31192,7 @@
     </row>
     <row r="83" spans="1:6" ht="15" customHeight="1">
       <c r="A83" s="83"/>
-      <c r="B83" s="200" t="s">
+      <c r="B83" s="202" t="s">
         <v>5223</v>
       </c>
       <c r="C83" t="s">
@@ -31194,7 +31204,7 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="83"/>
-      <c r="B84" s="200" t="s">
+      <c r="B84" s="202" t="s">
         <v>4459</v>
       </c>
       <c r="C84" t="s">
@@ -31206,7 +31216,7 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="83"/>
-      <c r="B85" s="200" t="s">
+      <c r="B85" s="202" t="s">
         <v>5688</v>
       </c>
       <c r="C85" t="s">
@@ -31218,7 +31228,7 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="83"/>
-      <c r="B86" s="200">
+      <c r="B86" s="202">
         <v>95368</v>
       </c>
       <c r="C86" t="s">
@@ -31232,7 +31242,7 @@
     </row>
     <row r="87" spans="1:6" ht="17.649999999999999" customHeight="1">
       <c r="A87" s="83"/>
-      <c r="B87" s="200" t="s">
+      <c r="B87" s="202" t="s">
         <v>4439</v>
       </c>
       <c r="C87" t="s">
@@ -31244,7 +31254,7 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="83"/>
-      <c r="B88" s="200" t="s">
+      <c r="B88" s="202" t="s">
         <v>168</v>
       </c>
       <c r="C88" t="s">
@@ -31256,7 +31266,7 @@
     </row>
     <row r="89" spans="1:6" ht="18" customHeight="1">
       <c r="A89" s="83"/>
-      <c r="B89" s="200" t="s">
+      <c r="B89" s="202" t="s">
         <v>995</v>
       </c>
       <c r="C89" t="s">
@@ -31272,7 +31282,7 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="83"/>
-      <c r="B90" s="200" t="s">
+      <c r="B90" s="202" t="s">
         <v>900</v>
       </c>
       <c r="C90" t="s">
@@ -31284,7 +31294,7 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="83"/>
-      <c r="B91" s="200" t="s">
+      <c r="B91" s="202" t="s">
         <v>177</v>
       </c>
       <c r="C91" t="s">
@@ -31298,7 +31308,7 @@
     </row>
     <row r="92" spans="1:6" ht="21.6" customHeight="1">
       <c r="A92" s="83"/>
-      <c r="B92" s="200" t="s">
+      <c r="B92" s="202" t="s">
         <v>4466</v>
       </c>
       <c r="C92" t="s">
@@ -31310,7 +31320,7 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="83"/>
-      <c r="B93" s="200">
+      <c r="B93" s="202">
         <v>70508</v>
       </c>
       <c r="C93" t="s">
@@ -31322,7 +31332,7 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="83"/>
-      <c r="B94" s="200" t="s">
+      <c r="B94" s="202" t="s">
         <v>4362</v>
       </c>
       <c r="C94" t="s">
@@ -31336,7 +31346,7 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="83"/>
-      <c r="B95" s="200" t="s">
+      <c r="B95" s="202" t="s">
         <v>4389</v>
       </c>
       <c r="C95" t="s">
@@ -31348,7 +31358,7 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="83"/>
-      <c r="B96" s="200">
+      <c r="B96" s="202">
         <v>32245</v>
       </c>
       <c r="C96" t="s">
@@ -31360,7 +31370,7 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="83"/>
-      <c r="B97" s="200" t="s">
+      <c r="B97" s="202" t="s">
         <v>922</v>
       </c>
       <c r="C97" t="s">
@@ -31374,7 +31384,7 @@
     </row>
     <row r="98" spans="1:6" ht="22.15" customHeight="1">
       <c r="A98" s="83"/>
-      <c r="B98" s="201" t="s">
+      <c r="B98" s="203" t="s">
         <v>4465</v>
       </c>
       <c r="C98" t="s">
@@ -31386,7 +31396,7 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="83"/>
-      <c r="B99" s="200" t="s">
+      <c r="B99" s="202" t="s">
         <v>655</v>
       </c>
       <c r="C99" t="s">
@@ -31400,7 +31410,7 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="83"/>
-      <c r="B100" s="200" t="s">
+      <c r="B100" s="202" t="s">
         <v>605</v>
       </c>
       <c r="C100" t="s">
@@ -31412,19 +31422,19 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="83"/>
-      <c r="B101" s="200" t="s">
+      <c r="B101" s="202" t="s">
         <v>4436</v>
       </c>
       <c r="C101" t="s">
         <v>4437</v>
       </c>
-      <c r="D101" s="197"/>
+      <c r="D101" s="198"/>
       <c r="E101" s="186"/>
       <c r="F101" s="83"/>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="83"/>
-      <c r="B102" s="200">
+      <c r="B102" s="202">
         <v>66618</v>
       </c>
       <c r="C102" t="s">
@@ -31438,7 +31448,7 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="83"/>
-      <c r="B103" s="200" t="s">
+      <c r="B103" s="202" t="s">
         <v>4282</v>
       </c>
       <c r="C103" t="s">
@@ -31452,7 +31462,7 @@
     </row>
     <row r="104" spans="1:6" ht="18" customHeight="1">
       <c r="A104" s="83"/>
-      <c r="B104" s="200" t="s">
+      <c r="B104" s="202" t="s">
         <v>5746</v>
       </c>
       <c r="C104" t="s">
@@ -31466,7 +31476,7 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="83"/>
-      <c r="B105" s="201" t="s">
+      <c r="B105" s="203" t="s">
         <v>5691</v>
       </c>
       <c r="C105" t="s">
@@ -31478,19 +31488,19 @@
     </row>
     <row r="106" spans="1:6" ht="16.149999999999999" customHeight="1">
       <c r="A106" s="83"/>
-      <c r="B106" s="200" t="s">
+      <c r="B106" s="202" t="s">
         <v>4452</v>
       </c>
       <c r="C106" t="s">
         <v>4453</v>
       </c>
       <c r="D106" s="186"/>
-      <c r="E106" s="197"/>
+      <c r="E106" s="198"/>
       <c r="F106" s="83"/>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="83"/>
-      <c r="B107" s="200" t="s">
+      <c r="B107" s="202" t="s">
         <v>4371</v>
       </c>
       <c r="C107" t="s">
@@ -31502,7 +31512,7 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="83"/>
-      <c r="B108" s="200" t="s">
+      <c r="B108" s="202" t="s">
         <v>5372</v>
       </c>
       <c r="C108" t="s">
@@ -31514,7 +31524,7 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="83"/>
-      <c r="B109" s="200" t="s">
+      <c r="B109" s="202" t="s">
         <v>4817</v>
       </c>
       <c r="C109" t="s">
@@ -31526,7 +31536,7 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="83"/>
-      <c r="B110" s="200" t="s">
+      <c r="B110" s="202" t="s">
         <v>442</v>
       </c>
       <c r="C110" t="s">
@@ -31535,12 +31545,12 @@
       <c r="D110" s="10" t="s">
         <v>1440</v>
       </c>
-      <c r="E110" s="197"/>
+      <c r="E110" s="198"/>
       <c r="F110" s="83"/>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="83"/>
-      <c r="B111" s="200">
+      <c r="B111" s="202">
         <v>86044</v>
       </c>
       <c r="C111" t="s">
@@ -31554,7 +31564,7 @@
     </row>
     <row r="112" spans="1:6" ht="16.149999999999999" customHeight="1">
       <c r="A112" s="83"/>
-      <c r="B112" s="200" t="s">
+      <c r="B112" s="202" t="s">
         <v>5845</v>
       </c>
       <c r="C112" t="s">
@@ -31568,7 +31578,7 @@
     </row>
     <row r="113" spans="1:6" ht="14.45" customHeight="1">
       <c r="A113" s="83"/>
-      <c r="B113" s="200" t="s">
+      <c r="B113" s="202" t="s">
         <v>403</v>
       </c>
       <c r="C113" t="s">
@@ -31580,7 +31590,7 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="83"/>
-      <c r="B114" s="200">
+      <c r="B114" s="202">
         <v>71304</v>
       </c>
       <c r="C114" t="s">
@@ -31592,7 +31602,7 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="83"/>
-      <c r="B115" s="200" t="s">
+      <c r="B115" s="202" t="s">
         <v>5428</v>
       </c>
       <c r="C115" t="s">
@@ -31604,7 +31614,7 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" s="83"/>
-      <c r="B116" s="200" t="s">
+      <c r="B116" s="202" t="s">
         <v>904</v>
       </c>
       <c r="C116" t="s">
@@ -31616,7 +31626,7 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="83"/>
-      <c r="B117" s="200">
+      <c r="B117" s="202">
         <v>65586</v>
       </c>
       <c r="C117" t="s">
@@ -31630,7 +31640,7 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="83"/>
-      <c r="B118" s="200" t="s">
+      <c r="B118" s="202" t="s">
         <v>5844</v>
       </c>
       <c r="C118" t="s">
@@ -31644,7 +31654,7 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="83"/>
-      <c r="B119" s="200" t="s">
+      <c r="B119" s="202" t="s">
         <v>1346</v>
       </c>
       <c r="C119" t="s">
@@ -31656,7 +31666,7 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" s="83"/>
-      <c r="B120" s="200">
+      <c r="B120" s="202">
         <v>54119</v>
       </c>
       <c r="C120" t="s">
@@ -31668,7 +31678,7 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" s="83"/>
-      <c r="B121" s="200">
+      <c r="B121" s="202">
         <v>10988</v>
       </c>
       <c r="C121" t="s">
@@ -31680,7 +31690,7 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="83"/>
-      <c r="B122" s="200">
+      <c r="B122" s="202">
         <v>81815</v>
       </c>
       <c r="C122" t="s">
@@ -31692,7 +31702,7 @@
     </row>
     <row r="123" spans="1:6" ht="18" customHeight="1">
       <c r="A123" s="83"/>
-      <c r="B123" s="200" t="s">
+      <c r="B123" s="202" t="s">
         <v>214</v>
       </c>
       <c r="C123" t="s">
@@ -31706,7 +31716,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" s="83"/>
-      <c r="B124" s="200" t="s">
+      <c r="B124" s="202" t="s">
         <v>4351</v>
       </c>
       <c r="C124" t="s">
@@ -31720,7 +31730,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" s="83"/>
-      <c r="B125" s="200" t="s">
+      <c r="B125" s="202" t="s">
         <v>4383</v>
       </c>
       <c r="C125" t="s">
@@ -31732,7 +31742,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" s="83"/>
-      <c r="B126" s="200">
+      <c r="B126" s="202">
         <v>15645</v>
       </c>
       <c r="C126" t="s">
@@ -31744,7 +31754,7 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" s="83"/>
-      <c r="B127" s="200">
+      <c r="B127" s="202">
         <v>76588</v>
       </c>
       <c r="C127" t="s">
@@ -31756,7 +31766,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" s="83"/>
-      <c r="B128" s="200" t="s">
+      <c r="B128" s="202" t="s">
         <v>1020</v>
       </c>
       <c r="C128" t="s">
@@ -31770,7 +31780,7 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" s="83"/>
-      <c r="B129" s="200">
+      <c r="B129" s="202">
         <v>11243</v>
       </c>
       <c r="C129" t="s">
@@ -31782,7 +31792,7 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" s="83"/>
-      <c r="B130" s="200" t="s">
+      <c r="B130" s="202" t="s">
         <v>631</v>
       </c>
       <c r="C130" t="s">
@@ -31796,7 +31806,7 @@
     </row>
     <row r="131" spans="1:6" ht="14.25" customHeight="1">
       <c r="A131" s="83"/>
-      <c r="B131" s="200" t="s">
+      <c r="B131" s="202" t="s">
         <v>1076</v>
       </c>
       <c r="C131" t="s">
@@ -31808,7 +31818,7 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" s="83"/>
-      <c r="B132" s="200">
+      <c r="B132" s="202">
         <v>66087</v>
       </c>
       <c r="C132" t="s">
@@ -31822,7 +31832,7 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" s="83"/>
-      <c r="B133" s="200" t="s">
+      <c r="B133" s="202" t="s">
         <v>532</v>
       </c>
       <c r="C133" t="s">
@@ -31836,7 +31846,7 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" s="83"/>
-      <c r="B134" s="200" t="s">
+      <c r="B134" s="202" t="s">
         <v>163</v>
       </c>
       <c r="C134" t="s">
@@ -31850,7 +31860,7 @@
     </row>
     <row r="135" spans="1:6" ht="19.5" customHeight="1">
       <c r="A135" s="83"/>
-      <c r="B135" s="200" t="s">
+      <c r="B135" s="202" t="s">
         <v>1311</v>
       </c>
       <c r="C135" t="s">
@@ -31862,7 +31872,7 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" s="83"/>
-      <c r="B136" s="200" t="s">
+      <c r="B136" s="202" t="s">
         <v>94</v>
       </c>
       <c r="C136" t="s">
@@ -31876,7 +31886,7 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" s="83"/>
-      <c r="B137" s="200">
+      <c r="B137" s="202">
         <v>71985</v>
       </c>
       <c r="C137" t="s">
@@ -31888,7 +31898,7 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" s="83"/>
-      <c r="B138" s="200" t="s">
+      <c r="B138" s="202" t="s">
         <v>4397</v>
       </c>
       <c r="C138" t="s">
@@ -31900,7 +31910,7 @@
     </row>
     <row r="139" spans="1:6" ht="18" customHeight="1">
       <c r="A139" s="83"/>
-      <c r="B139" s="200">
+      <c r="B139" s="202">
         <v>57771</v>
       </c>
       <c r="C139" t="s">
@@ -31912,7 +31922,7 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="83"/>
-      <c r="B140" s="200" t="s">
+      <c r="B140" s="202" t="s">
         <v>5370</v>
       </c>
       <c r="C140" t="s">
@@ -31924,7 +31934,7 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" s="83"/>
-      <c r="B141" s="200">
+      <c r="B141" s="202">
         <v>12190</v>
       </c>
       <c r="C141" t="s">
@@ -31936,7 +31946,7 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="83"/>
-      <c r="B142" s="200" t="s">
+      <c r="B142" s="202" t="s">
         <v>4486</v>
       </c>
       <c r="C142" t="s">
@@ -31948,7 +31958,7 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" s="83"/>
-      <c r="B143" s="200" t="s">
+      <c r="B143" s="202" t="s">
         <v>1181</v>
       </c>
       <c r="C143" t="s">
@@ -31962,7 +31972,7 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="83"/>
-      <c r="B144" s="200">
+      <c r="B144" s="202">
         <v>83533</v>
       </c>
       <c r="C144" t="s">
@@ -31976,7 +31986,7 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="83"/>
-      <c r="B145" s="200" t="s">
+      <c r="B145" s="202" t="s">
         <v>745</v>
       </c>
       <c r="C145" t="s">
@@ -31988,7 +31998,7 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="83"/>
-      <c r="B146" s="200" t="s">
+      <c r="B146" s="202" t="s">
         <v>5424</v>
       </c>
       <c r="C146" t="s">
@@ -32000,7 +32010,7 @@
     </row>
     <row r="147" spans="1:6" ht="19.5" customHeight="1">
       <c r="A147" s="83"/>
-      <c r="B147" s="200" t="s">
+      <c r="B147" s="202" t="s">
         <v>4249</v>
       </c>
       <c r="C147" t="s">
@@ -32012,7 +32022,7 @@
     </row>
     <row r="148" spans="1:6" ht="17.25" customHeight="1">
       <c r="A148" s="83"/>
-      <c r="B148" s="200" t="s">
+      <c r="B148" s="202" t="s">
         <v>4462</v>
       </c>
       <c r="C148" t="s">
@@ -32024,7 +32034,7 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" s="83"/>
-      <c r="B149" s="200" t="s">
+      <c r="B149" s="202" t="s">
         <v>4251</v>
       </c>
       <c r="C149" t="s">
@@ -32038,7 +32048,7 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" s="83"/>
-      <c r="B150" s="200" t="s">
+      <c r="B150" s="202" t="s">
         <v>507</v>
       </c>
       <c r="C150" t="s">
@@ -32050,7 +32060,7 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" s="83"/>
-      <c r="B151" s="200" t="s">
+      <c r="B151" s="202" t="s">
         <v>1522</v>
       </c>
       <c r="C151" t="s">
@@ -32064,7 +32074,7 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" s="83"/>
-      <c r="B152" s="200">
+      <c r="B152" s="202">
         <v>30169</v>
       </c>
       <c r="C152" t="s">
@@ -32076,7 +32086,7 @@
     </row>
     <row r="153" spans="1:6" ht="15.75" customHeight="1">
       <c r="A153" s="83"/>
-      <c r="B153" s="200" t="s">
+      <c r="B153" s="202" t="s">
         <v>4399</v>
       </c>
       <c r="C153" t="s">
@@ -32088,7 +32098,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="83"/>
-      <c r="B154" s="200" t="s">
+      <c r="B154" s="202" t="s">
         <v>4813</v>
       </c>
       <c r="C154" t="s">
@@ -32100,7 +32110,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" s="83"/>
-      <c r="B155" s="200" t="s">
+      <c r="B155" s="202" t="s">
         <v>4254</v>
       </c>
       <c r="C155" t="s">
@@ -32114,7 +32124,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" s="83"/>
-      <c r="B156" s="200">
+      <c r="B156" s="202">
         <v>73680</v>
       </c>
       <c r="C156" t="s">
@@ -32126,7 +32136,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="83"/>
-      <c r="B157" s="200" t="s">
+      <c r="B157" s="202" t="s">
         <v>4405</v>
       </c>
       <c r="C157" t="s">
@@ -32138,7 +32148,7 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" s="83"/>
-      <c r="B158" s="200" t="s">
+      <c r="B158" s="202" t="s">
         <v>4356</v>
       </c>
       <c r="C158" t="s">
@@ -32150,7 +32160,7 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="83"/>
-      <c r="B159" s="200" t="s">
+      <c r="B159" s="202" t="s">
         <v>4257</v>
       </c>
       <c r="C159" t="s">
@@ -32164,7 +32174,7 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="83"/>
-      <c r="B160" s="200" t="s">
+      <c r="B160" s="202" t="s">
         <v>4260</v>
       </c>
       <c r="C160" t="s">
@@ -32178,7 +32188,7 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="83"/>
-      <c r="B161" s="200">
+      <c r="B161" s="202">
         <v>63282</v>
       </c>
       <c r="C161" t="s">
@@ -32190,7 +32200,7 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" s="83"/>
-      <c r="B162" s="200">
+      <c r="B162" s="202">
         <v>52213</v>
       </c>
       <c r="C162" t="s">
@@ -32202,7 +32212,7 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="83"/>
-      <c r="B163" s="200" t="s">
+      <c r="B163" s="202" t="s">
         <v>612</v>
       </c>
       <c r="C163" t="s">
@@ -32216,7 +32226,7 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="83"/>
-      <c r="B164" s="200" t="s">
+      <c r="B164" s="202" t="s">
         <v>4418</v>
       </c>
       <c r="C164" t="s">
@@ -32228,7 +32238,7 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="83"/>
-      <c r="B165" s="200" t="s">
+      <c r="B165" s="202" t="s">
         <v>5840</v>
       </c>
       <c r="C165" t="s">
@@ -32240,7 +32250,7 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="83"/>
-      <c r="B166" s="200" t="s">
+      <c r="B166" s="202" t="s">
         <v>4405</v>
       </c>
       <c r="C166" t="s">
@@ -32252,7 +32262,7 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="83"/>
-      <c r="B167" s="200">
+      <c r="B167" s="202">
         <v>53882</v>
       </c>
       <c r="C167" t="s">
@@ -32264,7 +32274,7 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="83"/>
-      <c r="B168" s="200" t="s">
+      <c r="B168" s="202" t="s">
         <v>5847</v>
       </c>
       <c r="C168" t="s">
@@ -32278,7 +32288,7 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="83"/>
-      <c r="B169" s="200">
+      <c r="B169" s="202">
         <v>64411</v>
       </c>
       <c r="C169" t="s">
@@ -32290,7 +32300,7 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="83"/>
-      <c r="B170" s="200">
+      <c r="B170" s="202">
         <v>34222</v>
       </c>
       <c r="C170" t="s">
@@ -32302,7 +32312,7 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="83"/>
-      <c r="B171" s="200" t="s">
+      <c r="B171" s="202" t="s">
         <v>5841</v>
       </c>
       <c r="C171" t="s">
@@ -32316,7 +32326,7 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="83"/>
-      <c r="B172" s="200" t="s">
+      <c r="B172" s="202" t="s">
         <v>1170</v>
       </c>
       <c r="C172" t="s">
@@ -32330,7 +32340,7 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="83"/>
-      <c r="B173" s="200" t="s">
+      <c r="B173" s="202" t="s">
         <v>5823</v>
       </c>
       <c r="C173" t="s">
@@ -32342,7 +32352,7 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="83"/>
-      <c r="B174" s="200" t="s">
+      <c r="B174" s="202" t="s">
         <v>408</v>
       </c>
       <c r="C174" t="s">
@@ -32356,7 +32366,7 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" s="83"/>
-      <c r="B175" s="200" t="s">
+      <c r="B175" s="202" t="s">
         <v>97</v>
       </c>
       <c r="C175" t="s">
@@ -32368,7 +32378,7 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" s="83"/>
-      <c r="B176" s="200" t="s">
+      <c r="B176" s="202" t="s">
         <v>4340</v>
       </c>
       <c r="C176" t="s">
@@ -32380,7 +32390,7 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" s="83"/>
-      <c r="B177" s="200">
+      <c r="B177" s="202">
         <v>11707</v>
       </c>
       <c r="C177" t="s">
@@ -32392,7 +32402,7 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" s="83"/>
-      <c r="B178" s="200" t="s">
+      <c r="B178" s="202" t="s">
         <v>5419</v>
       </c>
       <c r="C178" t="s">
@@ -32404,7 +32414,7 @@
     </row>
     <row r="179" spans="1:6" ht="18" customHeight="1">
       <c r="A179" s="83"/>
-      <c r="B179" s="200" t="s">
+      <c r="B179" s="202" t="s">
         <v>513</v>
       </c>
       <c r="C179" t="s">
@@ -32416,7 +32426,7 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" s="83"/>
-      <c r="B180" s="200" t="s">
+      <c r="B180" s="202" t="s">
         <v>5677</v>
       </c>
       <c r="C180" t="s">
@@ -32428,7 +32438,7 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" s="83"/>
-      <c r="B181" s="200" t="s">
+      <c r="B181" s="202" t="s">
         <v>5687</v>
       </c>
       <c r="C181" t="s">
@@ -32440,7 +32450,7 @@
     </row>
     <row r="182" spans="1:6">
       <c r="A182" s="83"/>
-      <c r="B182" s="200" t="s">
+      <c r="B182" s="202" t="s">
         <v>4408</v>
       </c>
       <c r="C182" t="s">
@@ -32452,7 +32462,7 @@
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="83"/>
-      <c r="B183" s="200" t="s">
+      <c r="B183" s="202" t="s">
         <v>228</v>
       </c>
       <c r="C183" t="s">
@@ -32466,7 +32476,7 @@
     </row>
     <row r="184" spans="1:6">
       <c r="A184" s="83"/>
-      <c r="B184" s="201" t="s">
+      <c r="B184" s="203" t="s">
         <v>4467</v>
       </c>
       <c r="C184" t="s">
@@ -32478,7 +32488,7 @@
     </row>
     <row r="185" spans="1:6">
       <c r="A185" s="83"/>
-      <c r="B185" s="200">
+      <c r="B185" s="202">
         <v>71670</v>
       </c>
       <c r="C185" t="s">
@@ -32490,7 +32500,7 @@
     </row>
     <row r="186" spans="1:6">
       <c r="A186" s="83"/>
-      <c r="B186" s="200">
+      <c r="B186" s="202">
         <v>26136</v>
       </c>
       <c r="C186" t="s">
@@ -32502,7 +32512,7 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" s="83"/>
-      <c r="B187" s="200" t="s">
+      <c r="B187" s="202" t="s">
         <v>4432</v>
       </c>
       <c r="C187" t="s">
@@ -32514,7 +32524,7 @@
     </row>
     <row r="188" spans="1:6">
       <c r="A188" s="83"/>
-      <c r="B188" s="200" t="s">
+      <c r="B188" s="202" t="s">
         <v>898</v>
       </c>
       <c r="C188" t="s">
@@ -32528,7 +32538,7 @@
     </row>
     <row r="189" spans="1:6">
       <c r="A189" s="83"/>
-      <c r="B189" s="200" t="s">
+      <c r="B189" s="202" t="s">
         <v>4434</v>
       </c>
       <c r="C189" t="s">
@@ -32540,7 +32550,7 @@
     </row>
     <row r="190" spans="1:6">
       <c r="A190" s="83"/>
-      <c r="B190" s="200">
+      <c r="B190" s="202">
         <v>85213</v>
       </c>
       <c r="C190" t="s">
@@ -32554,7 +32564,7 @@
     </row>
     <row r="191" spans="1:6">
       <c r="A191" s="83"/>
-      <c r="B191" s="200">
+      <c r="B191" s="202">
         <v>95094</v>
       </c>
       <c r="C191" t="s">
@@ -32566,7 +32576,7 @@
     </row>
     <row r="192" spans="1:6" ht="13.5" customHeight="1">
       <c r="A192" s="83"/>
-      <c r="B192" s="200">
+      <c r="B192" s="202">
         <v>33152</v>
       </c>
       <c r="C192" t="s">
@@ -32578,7 +32588,7 @@
     </row>
     <row r="193" spans="1:6">
       <c r="A193" s="83"/>
-      <c r="B193" s="200">
+      <c r="B193" s="202">
         <v>17798</v>
       </c>
       <c r="C193" t="s">
@@ -32590,7 +32600,7 @@
     </row>
     <row r="194" spans="1:6" ht="17.45" customHeight="1">
       <c r="A194" s="83"/>
-      <c r="B194" s="200" t="s">
+      <c r="B194" s="202" t="s">
         <v>582</v>
       </c>
       <c r="C194" t="s">
@@ -32604,7 +32614,7 @@
     </row>
     <row r="195" spans="1:6" ht="17.25" customHeight="1">
       <c r="A195" s="83"/>
-      <c r="B195" s="200" t="s">
+      <c r="B195" s="202" t="s">
         <v>282</v>
       </c>
       <c r="C195" t="s">
@@ -32616,7 +32626,7 @@
     </row>
     <row r="196" spans="1:6">
       <c r="A196" s="83"/>
-      <c r="B196" s="200" t="s">
+      <c r="B196" s="202" t="s">
         <v>5835</v>
       </c>
       <c r="C196" t="s">
@@ -32628,7 +32638,7 @@
     </row>
     <row r="197" spans="1:6">
       <c r="A197" s="83"/>
-      <c r="B197" s="200" t="s">
+      <c r="B197" s="202" t="s">
         <v>4355</v>
       </c>
       <c r="C197" t="s">
@@ -32640,7 +32650,7 @@
     </row>
     <row r="198" spans="1:6">
       <c r="A198" s="83"/>
-      <c r="B198" s="200" t="s">
+      <c r="B198" s="202" t="s">
         <v>1865</v>
       </c>
       <c r="C198" t="s">
@@ -32654,7 +32664,7 @@
     </row>
     <row r="199" spans="1:6">
       <c r="A199" s="83"/>
-      <c r="B199" s="200">
+      <c r="B199" s="202">
         <v>14561</v>
       </c>
       <c r="C199" t="s">
@@ -32666,7 +32676,7 @@
     </row>
     <row r="200" spans="1:6">
       <c r="A200" s="83"/>
-      <c r="B200" s="200">
+      <c r="B200" s="202">
         <v>87009</v>
       </c>
       <c r="C200" t="s">
@@ -32678,7 +32688,7 @@
     </row>
     <row r="201" spans="1:6">
       <c r="A201" s="83"/>
-      <c r="B201" s="200">
+      <c r="B201" s="202">
         <v>38664</v>
       </c>
       <c r="C201" t="s">
@@ -32690,7 +32700,7 @@
     </row>
     <row r="202" spans="1:6">
       <c r="A202" s="83"/>
-      <c r="B202" s="200">
+      <c r="B202" s="202">
         <v>60955</v>
       </c>
       <c r="C202" t="s">
@@ -32704,7 +32714,7 @@
     </row>
     <row r="203" spans="1:6">
       <c r="A203" s="83"/>
-      <c r="B203" s="200">
+      <c r="B203" s="202">
         <v>13047</v>
       </c>
       <c r="C203" t="s">
@@ -32718,7 +32728,7 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="83"/>
-      <c r="B204" s="200">
+      <c r="B204" s="202">
         <v>22978</v>
       </c>
       <c r="C204" t="s">
@@ -32732,7 +32742,7 @@
     </row>
     <row r="205" spans="1:6">
       <c r="A205" s="83"/>
-      <c r="B205" s="200" t="s">
+      <c r="B205" s="202" t="s">
         <v>5236</v>
       </c>
       <c r="C205" t="s">
@@ -32744,7 +32754,7 @@
     </row>
     <row r="206" spans="1:6">
       <c r="A206" s="83"/>
-      <c r="B206" s="200">
+      <c r="B206" s="202">
         <v>12021</v>
       </c>
       <c r="C206" t="s">
@@ -32756,7 +32766,7 @@
     </row>
     <row r="207" spans="1:6">
       <c r="A207" s="83"/>
-      <c r="B207" s="200">
+      <c r="B207" s="202">
         <v>62727</v>
       </c>
       <c r="C207" t="s">
@@ -32770,7 +32780,7 @@
     </row>
     <row r="208" spans="1:6">
       <c r="A208" s="83"/>
-      <c r="B208" s="200" t="s">
+      <c r="B208" s="202" t="s">
         <v>1689</v>
       </c>
       <c r="C208" t="s">
@@ -32784,7 +32794,7 @@
     </row>
     <row r="209" spans="1:6">
       <c r="A209" s="83"/>
-      <c r="B209" s="200" t="s">
+      <c r="B209" s="202" t="s">
         <v>4275</v>
       </c>
       <c r="C209" t="s">
@@ -32798,7 +32808,7 @@
     </row>
     <row r="210" spans="1:6">
       <c r="A210" s="83"/>
-      <c r="B210" s="200" t="s">
+      <c r="B210" s="202" t="s">
         <v>4455</v>
       </c>
       <c r="C210" t="s">
@@ -32810,7 +32820,7 @@
     </row>
     <row r="211" spans="1:6" ht="18.75" customHeight="1">
       <c r="A211" s="83"/>
-      <c r="B211" s="200">
+      <c r="B211" s="202">
         <v>38881</v>
       </c>
       <c r="C211" t="s">
@@ -32822,7 +32832,7 @@
     </row>
     <row r="212" spans="1:6">
       <c r="A212" s="83"/>
-      <c r="B212" s="200">
+      <c r="B212" s="202">
         <v>41592</v>
       </c>
       <c r="C212" t="s">
@@ -32834,7 +32844,7 @@
     </row>
     <row r="213" spans="1:6" ht="18" customHeight="1">
       <c r="A213" s="83"/>
-      <c r="B213" s="200" t="s">
+      <c r="B213" s="202" t="s">
         <v>4470</v>
       </c>
       <c r="C213" t="s">
@@ -32846,7 +32856,7 @@
     </row>
     <row r="214" spans="1:6">
       <c r="A214" s="83"/>
-      <c r="B214" s="200" t="s">
+      <c r="B214" s="202" t="s">
         <v>4489</v>
       </c>
       <c r="C214" t="s">
@@ -32858,7 +32868,7 @@
     </row>
     <row r="215" spans="1:6">
       <c r="A215" s="83"/>
-      <c r="B215" s="200">
+      <c r="B215" s="202">
         <v>32387</v>
       </c>
       <c r="C215" t="s">
@@ -32872,7 +32882,7 @@
     </row>
     <row r="216" spans="1:6">
       <c r="A216" s="83"/>
-      <c r="B216" s="200" t="s">
+      <c r="B216" s="202" t="s">
         <v>5837</v>
       </c>
       <c r="C216" t="s">
@@ -32884,7 +32894,7 @@
     </row>
     <row r="217" spans="1:6">
       <c r="A217" s="83"/>
-      <c r="B217" s="200"/>
+      <c r="B217" s="202"/>
       <c r="C217" t="s">
         <v>1565</v>
       </c>
@@ -32894,7 +32904,7 @@
     </row>
     <row r="218" spans="1:6">
       <c r="A218" s="83"/>
-      <c r="B218" s="200">
+      <c r="B218" s="202">
         <v>43990</v>
       </c>
       <c r="C218" t="s">
@@ -32906,7 +32916,7 @@
     </row>
     <row r="219" spans="1:6">
       <c r="A219" s="83"/>
-      <c r="B219" s="200">
+      <c r="B219" s="202">
         <v>59165</v>
       </c>
       <c r="C219" t="s">
@@ -32920,7 +32930,7 @@
     </row>
     <row r="220" spans="1:6">
       <c r="A220" s="83"/>
-      <c r="B220" s="200" t="s">
+      <c r="B220" s="202" t="s">
         <v>676</v>
       </c>
       <c r="C220" t="s">
@@ -32934,7 +32944,7 @@
     </row>
     <row r="221" spans="1:6">
       <c r="A221" s="83"/>
-      <c r="B221" s="200" t="s">
+      <c r="B221" s="202" t="s">
         <v>4802</v>
       </c>
       <c r="C221" t="s">
@@ -32946,7 +32956,7 @@
     </row>
     <row r="222" spans="1:6">
       <c r="A222" s="83"/>
-      <c r="B222" s="200" t="s">
+      <c r="B222" s="202" t="s">
         <v>4527</v>
       </c>
       <c r="C222" t="s">
@@ -32958,7 +32968,7 @@
     </row>
     <row r="223" spans="1:6">
       <c r="A223" s="83"/>
-      <c r="B223" s="200" t="s">
+      <c r="B223" s="202" t="s">
         <v>5685</v>
       </c>
       <c r="C223" t="s">
@@ -32970,7 +32980,7 @@
     </row>
     <row r="224" spans="1:6">
       <c r="A224" s="83"/>
-      <c r="B224" s="200">
+      <c r="B224" s="202">
         <v>25281</v>
       </c>
       <c r="C224" t="s">
@@ -32982,7 +32992,7 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" s="83"/>
-      <c r="B225" s="200">
+      <c r="B225" s="202">
         <v>12066</v>
       </c>
       <c r="C225" t="s">
@@ -32994,7 +33004,7 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" s="83"/>
-      <c r="B226" s="200" t="s">
+      <c r="B226" s="202" t="s">
         <v>5836</v>
       </c>
       <c r="C226" t="s">
@@ -33006,7 +33016,7 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" s="83"/>
-      <c r="B227" s="200">
+      <c r="B227" s="202">
         <v>44674</v>
       </c>
       <c r="C227" t="s">
@@ -33018,7 +33028,7 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" s="83"/>
-      <c r="B228" s="200">
+      <c r="B228" s="202">
         <v>34712</v>
       </c>
       <c r="C228" t="s">
@@ -33030,7 +33040,7 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" s="83"/>
-      <c r="B229" s="200">
+      <c r="B229" s="202">
         <v>15305</v>
       </c>
       <c r="C229" t="s">
@@ -33042,7 +33052,7 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" s="83"/>
-      <c r="B230" s="200">
+      <c r="B230" s="202">
         <v>63266</v>
       </c>
       <c r="C230" t="s">
@@ -33054,7 +33064,7 @@
     </row>
     <row r="231" spans="1:6">
       <c r="A231" s="83"/>
-      <c r="B231" s="200" t="s">
+      <c r="B231" s="202" t="s">
         <v>5238</v>
       </c>
       <c r="C231" t="s">
@@ -33066,7 +33076,7 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" s="83"/>
-      <c r="B232" s="200" t="s">
+      <c r="B232" s="202" t="s">
         <v>487</v>
       </c>
       <c r="C232" t="s">
@@ -33080,7 +33090,7 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" s="83"/>
-      <c r="B233" s="200" t="s">
+      <c r="B233" s="202" t="s">
         <v>608</v>
       </c>
       <c r="C233" t="s">
@@ -33094,7 +33104,7 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" s="83"/>
-      <c r="B234" s="200" t="s">
+      <c r="B234" s="202" t="s">
         <v>5450</v>
       </c>
       <c r="C234" t="s">
@@ -33106,7 +33116,7 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="83"/>
-      <c r="B235" s="200">
+      <c r="B235" s="202">
         <v>66774</v>
       </c>
       <c r="C235" t="s">
@@ -33118,7 +33128,7 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" s="83"/>
-      <c r="B236" s="200" t="s">
+      <c r="B236" s="202" t="s">
         <v>5421</v>
       </c>
       <c r="C236" t="s">
@@ -33130,7 +33140,7 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" s="83"/>
-      <c r="B237" s="200" t="s">
+      <c r="B237" s="202" t="s">
         <v>4449</v>
       </c>
       <c r="C237" t="s">
@@ -33142,7 +33152,7 @@
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="83"/>
-      <c r="B238" s="200" t="s">
+      <c r="B238" s="202" t="s">
         <v>4295</v>
       </c>
       <c r="C238" t="s">
@@ -33156,7 +33166,7 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="83"/>
-      <c r="B239" s="200">
+      <c r="B239" s="202">
         <v>63208</v>
       </c>
       <c r="C239" t="s">
@@ -33168,7 +33178,7 @@
     </row>
     <row r="240" spans="1:6">
       <c r="A240" s="83"/>
-      <c r="B240" s="200">
+      <c r="B240" s="202">
         <v>90031</v>
       </c>
       <c r="C240" t="s">
@@ -33180,7 +33190,7 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" s="83"/>
-      <c r="B241" s="201" t="s">
+      <c r="B241" s="203" t="s">
         <v>5834</v>
       </c>
       <c r="C241" t="s">
@@ -33192,7 +33202,7 @@
     </row>
     <row r="242" spans="1:6">
       <c r="A242" s="83"/>
-      <c r="B242" s="200">
+      <c r="B242" s="202">
         <v>54584</v>
       </c>
       <c r="C242" t="s">
@@ -33204,7 +33214,7 @@
     </row>
     <row r="243" spans="1:6">
       <c r="A243" s="83"/>
-      <c r="B243" s="200" t="s">
+      <c r="B243" s="202" t="s">
         <v>4447</v>
       </c>
       <c r="C243" t="s">
@@ -33216,7 +33226,7 @@
     </row>
     <row r="244" spans="1:6">
       <c r="A244" s="83"/>
-      <c r="B244" s="200">
+      <c r="B244" s="202">
         <v>52406</v>
       </c>
       <c r="C244" t="s">
@@ -33227,7 +33237,7 @@
       <c r="F244" s="83"/>
     </row>
     <row r="245" spans="1:6">
-      <c r="B245" s="200">
+      <c r="B245" s="202">
         <v>86835</v>
       </c>
       <c r="C245" t="s">
@@ -33241,7 +33251,7 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" s="83"/>
-      <c r="B246" s="200" t="s">
+      <c r="B246" s="202" t="s">
         <v>5714</v>
       </c>
       <c r="C246" t="s">
@@ -33253,7 +33263,7 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" s="83"/>
-      <c r="B247" s="200">
+      <c r="B247" s="202">
         <v>86928</v>
       </c>
       <c r="C247" t="s">
@@ -33265,7 +33275,7 @@
     </row>
     <row r="248" spans="1:6">
       <c r="A248" s="83"/>
-      <c r="B248" s="200">
+      <c r="B248" s="202">
         <v>9704</v>
       </c>
       <c r="C248" t="s">
@@ -33277,7 +33287,7 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" s="83"/>
-      <c r="B249" s="200">
+      <c r="B249" s="202">
         <v>91643</v>
       </c>
       <c r="C249" t="s">
@@ -33289,7 +33299,7 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" s="83"/>
-      <c r="B250" s="200" t="s">
+      <c r="B250" s="202" t="s">
         <v>5838</v>
       </c>
       <c r="C250" t="s">
@@ -33301,7 +33311,7 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="83"/>
-      <c r="B251" s="200" t="s">
+      <c r="B251" s="202" t="s">
         <v>5828</v>
       </c>
       <c r="C251" t="s">
@@ -33313,7 +33323,7 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" s="83"/>
-      <c r="B252" s="200" t="s">
+      <c r="B252" s="202" t="s">
         <v>4344</v>
       </c>
       <c r="C252" t="s">
@@ -33325,7 +33335,7 @@
     </row>
     <row r="253" spans="1:6">
       <c r="A253" s="83"/>
-      <c r="B253" s="200" t="s">
+      <c r="B253" s="202" t="s">
         <v>4822</v>
       </c>
       <c r="C253" t="s">
@@ -33337,7 +33347,7 @@
     </row>
     <row r="254" spans="1:6">
       <c r="A254" s="83"/>
-      <c r="B254" s="200" t="s">
+      <c r="B254" s="202" t="s">
         <v>5750</v>
       </c>
       <c r="C254" t="s">
@@ -33349,7 +33359,7 @@
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="83"/>
-      <c r="B255" s="200">
+      <c r="B255" s="202">
         <v>78359</v>
       </c>
       <c r="C255" t="s">
@@ -33361,7 +33371,7 @@
     </row>
     <row r="256" spans="1:6">
       <c r="A256" s="83"/>
-      <c r="B256" s="200">
+      <c r="B256" s="202">
         <v>28818</v>
       </c>
       <c r="C256" t="s">
@@ -33373,7 +33383,7 @@
     </row>
     <row r="257" spans="1:6">
       <c r="A257" s="83"/>
-      <c r="B257" s="200" t="s">
+      <c r="B257" s="202" t="s">
         <v>501</v>
       </c>
       <c r="C257" t="s">
@@ -33387,7 +33397,7 @@
     </row>
     <row r="258" spans="1:6">
       <c r="A258" s="83"/>
-      <c r="B258" s="200">
+      <c r="B258" s="202">
         <v>80756</v>
       </c>
       <c r="C258" t="s">
@@ -33399,7 +33409,7 @@
     </row>
     <row r="259" spans="1:6">
       <c r="A259" s="83"/>
-      <c r="B259" s="200">
+      <c r="B259" s="202">
         <v>66144</v>
       </c>
       <c r="C259" t="s">
@@ -33411,7 +33421,7 @@
     </row>
     <row r="260" spans="1:6">
       <c r="A260" s="83"/>
-      <c r="B260" s="200" t="s">
+      <c r="B260" s="202" t="s">
         <v>4407</v>
       </c>
       <c r="C260" t="s">
@@ -33423,7 +33433,7 @@
     </row>
     <row r="261" spans="1:6">
       <c r="A261" s="83"/>
-      <c r="B261" s="200">
+      <c r="B261" s="202">
         <v>98376</v>
       </c>
       <c r="C261" t="s">
@@ -33435,7 +33445,7 @@
     </row>
     <row r="262" spans="1:6">
       <c r="A262" s="83"/>
-      <c r="B262" s="200" t="s">
+      <c r="B262" s="202" t="s">
         <v>4804</v>
       </c>
       <c r="C262" t="s">
@@ -33447,7 +33457,7 @@
     </row>
     <row r="263" spans="1:6">
       <c r="A263" s="83"/>
-      <c r="B263" s="200">
+      <c r="B263" s="202">
         <v>15939</v>
       </c>
       <c r="C263" t="s">
@@ -33459,7 +33469,7 @@
     </row>
     <row r="264" spans="1:6">
       <c r="A264" s="83"/>
-      <c r="B264" s="200" t="s">
+      <c r="B264" s="202" t="s">
         <v>4639</v>
       </c>
       <c r="C264" t="s">
@@ -33471,7 +33481,7 @@
     </row>
     <row r="265" spans="1:6">
       <c r="A265" s="83"/>
-      <c r="B265" s="200" t="s">
+      <c r="B265" s="202" t="s">
         <v>4302</v>
       </c>
       <c r="C265" t="s">
@@ -33485,7 +33495,7 @@
     </row>
     <row r="266" spans="1:6">
       <c r="A266" s="83"/>
-      <c r="B266" s="200" t="s">
+      <c r="B266" s="202" t="s">
         <v>4821</v>
       </c>
       <c r="C266" t="s">
@@ -33497,7 +33507,7 @@
     </row>
     <row r="267" spans="1:6">
       <c r="A267" s="83"/>
-      <c r="B267" s="200" t="s">
+      <c r="B267" s="202" t="s">
         <v>4305</v>
       </c>
       <c r="C267" t="s">
@@ -33511,7 +33521,7 @@
     </row>
     <row r="268" spans="1:6">
       <c r="A268" s="83"/>
-      <c r="B268" s="200">
+      <c r="B268" s="202">
         <v>59529</v>
       </c>
       <c r="C268" t="s">
@@ -33523,7 +33533,7 @@
     </row>
     <row r="269" spans="1:6">
       <c r="A269" s="83"/>
-      <c r="B269" s="200" t="s">
+      <c r="B269" s="202" t="s">
         <v>4392</v>
       </c>
       <c r="C269" t="s">
@@ -33535,7 +33545,7 @@
     </row>
     <row r="270" spans="1:6">
       <c r="A270" s="83"/>
-      <c r="B270" s="200">
+      <c r="B270" s="202">
         <v>29019</v>
       </c>
       <c r="C270" t="s">
@@ -33547,7 +33557,7 @@
     </row>
     <row r="271" spans="1:6">
       <c r="A271" s="83"/>
-      <c r="B271" s="200" t="s">
+      <c r="B271" s="202" t="s">
         <v>5857</v>
       </c>
       <c r="C271" t="s">
@@ -33559,7 +33569,7 @@
     </row>
     <row r="272" spans="1:6">
       <c r="A272" s="83"/>
-      <c r="B272" s="200">
+      <c r="B272" s="202">
         <v>33476</v>
       </c>
       <c r="C272" t="s">
@@ -33571,7 +33581,7 @@
     </row>
     <row r="273" spans="1:6" ht="15.75" customHeight="1">
       <c r="A273" s="83"/>
-      <c r="B273" s="200" t="s">
+      <c r="B273" s="202" t="s">
         <v>1204</v>
       </c>
       <c r="C273" t="s">
@@ -33583,7 +33593,7 @@
     </row>
     <row r="274" spans="1:6">
       <c r="A274" s="83"/>
-      <c r="B274" s="200">
+      <c r="B274" s="202">
         <v>64023</v>
       </c>
       <c r="C274" t="s">
@@ -33597,7 +33607,7 @@
     </row>
     <row r="275" spans="1:6">
       <c r="A275" s="83"/>
-      <c r="B275" s="200" t="s">
+      <c r="B275" s="202" t="s">
         <v>374</v>
       </c>
       <c r="C275" t="s">
@@ -33609,7 +33619,7 @@
     </row>
     <row r="276" spans="1:6">
       <c r="A276" s="83"/>
-      <c r="B276" s="200">
+      <c r="B276" s="202">
         <v>64413</v>
       </c>
       <c r="C276" t="s">
@@ -33621,7 +33631,7 @@
     </row>
     <row r="277" spans="1:6">
       <c r="A277" s="83"/>
-      <c r="B277" s="200" t="s">
+      <c r="B277" s="202" t="s">
         <v>376</v>
       </c>
       <c r="C277" t="s">
@@ -33633,7 +33643,7 @@
     </row>
     <row r="278" spans="1:6">
       <c r="A278" s="83"/>
-      <c r="B278" s="200" t="s">
+      <c r="B278" s="202" t="s">
         <v>5851</v>
       </c>
       <c r="C278" t="s">
@@ -33647,7 +33657,7 @@
     </row>
     <row r="279" spans="1:6">
       <c r="A279" s="83"/>
-      <c r="B279" s="200">
+      <c r="B279" s="202">
         <v>82689</v>
       </c>
       <c r="C279" t="s">
@@ -33659,7 +33669,7 @@
     </row>
     <row r="280" spans="1:6">
       <c r="A280" s="83"/>
-      <c r="B280" s="200">
+      <c r="B280" s="202">
         <v>82402</v>
       </c>
       <c r="C280" t="s">
@@ -33671,7 +33681,7 @@
     </row>
     <row r="281" spans="1:6">
       <c r="A281" s="83"/>
-      <c r="B281" s="200" t="s">
+      <c r="B281" s="202" t="s">
         <v>1140</v>
       </c>
       <c r="C281" t="s">
@@ -33683,7 +33693,7 @@
     </row>
     <row r="282" spans="1:6">
       <c r="A282" s="83"/>
-      <c r="B282" s="200" t="s">
+      <c r="B282" s="202" t="s">
         <v>4451</v>
       </c>
       <c r="C282" t="s">
@@ -33695,7 +33705,7 @@
     </row>
     <row r="283" spans="1:6">
       <c r="A283" s="83"/>
-      <c r="B283" s="200">
+      <c r="B283" s="202">
         <v>48104</v>
       </c>
       <c r="C283" t="s">
@@ -33707,7 +33717,7 @@
     </row>
     <row r="284" spans="1:6">
       <c r="A284" s="83"/>
-      <c r="B284" s="200" t="s">
+      <c r="B284" s="202" t="s">
         <v>4441</v>
       </c>
       <c r="C284" t="s">
@@ -33721,7 +33731,7 @@
     </row>
     <row r="285" spans="1:6">
       <c r="A285" s="83"/>
-      <c r="B285" s="200" t="s">
+      <c r="B285" s="202" t="s">
         <v>5853</v>
       </c>
       <c r="C285" t="s">
@@ -33733,7 +33743,7 @@
     </row>
     <row r="286" spans="1:6">
       <c r="A286" s="83"/>
-      <c r="B286" s="200" t="s">
+      <c r="B286" s="202" t="s">
         <v>5439</v>
       </c>
       <c r="C286" t="s">
@@ -33745,7 +33755,7 @@
     </row>
     <row r="287" spans="1:6">
       <c r="A287" s="83"/>
-      <c r="B287" s="200" t="s">
+      <c r="B287" s="202" t="s">
         <v>5743</v>
       </c>
       <c r="C287" t="s">
@@ -33757,7 +33767,7 @@
     </row>
     <row r="288" spans="1:6">
       <c r="A288" s="83"/>
-      <c r="B288" s="200">
+      <c r="B288" s="202">
         <v>25714</v>
       </c>
       <c r="C288" t="s">
@@ -33769,7 +33779,7 @@
     </row>
     <row r="289" spans="1:6">
       <c r="A289" s="83"/>
-      <c r="B289" s="200">
+      <c r="B289" s="202">
         <v>25714</v>
       </c>
       <c r="C289" t="s">
@@ -33781,7 +33791,7 @@
     </row>
     <row r="290" spans="1:6">
       <c r="A290" s="83"/>
-      <c r="B290" s="200" t="s">
+      <c r="B290" s="202" t="s">
         <v>4307</v>
       </c>
       <c r="C290" t="s">
@@ -33795,7 +33805,7 @@
     </row>
     <row r="291" spans="1:6">
       <c r="A291" s="83"/>
-      <c r="B291" s="200" t="s">
+      <c r="B291" s="202" t="s">
         <v>5856</v>
       </c>
       <c r="C291" t="s">
@@ -33807,7 +33817,7 @@
     </row>
     <row r="292" spans="1:6">
       <c r="A292" s="83"/>
-      <c r="B292" s="200" t="s">
+      <c r="B292" s="202" t="s">
         <v>5426</v>
       </c>
       <c r="C292" t="s">
@@ -33819,7 +33829,7 @@
     </row>
     <row r="293" spans="1:6">
       <c r="A293" s="83"/>
-      <c r="B293" s="200" t="s">
+      <c r="B293" s="202" t="s">
         <v>4410</v>
       </c>
       <c r="C293" t="s">
@@ -33831,7 +33841,7 @@
     </row>
     <row r="294" spans="1:6">
       <c r="A294" s="83"/>
-      <c r="B294" s="200" t="s">
+      <c r="B294" s="202" t="s">
         <v>4309</v>
       </c>
       <c r="C294" t="s">
@@ -33843,7 +33853,7 @@
     </row>
     <row r="295" spans="1:6">
       <c r="A295" s="83"/>
-      <c r="B295" s="200" t="s">
+      <c r="B295" s="202" t="s">
         <v>5854</v>
       </c>
       <c r="C295" t="s">
@@ -33857,7 +33867,7 @@
     </row>
     <row r="296" spans="1:6">
       <c r="A296" s="83"/>
-      <c r="B296" s="200">
+      <c r="B296" s="202">
         <v>71670</v>
       </c>
       <c r="C296" t="s">
@@ -33869,7 +33879,7 @@
     </row>
     <row r="297" spans="1:6">
       <c r="A297" s="83"/>
-      <c r="B297" s="200" t="s">
+      <c r="B297" s="202" t="s">
         <v>4811</v>
       </c>
       <c r="C297" t="s">
@@ -33881,7 +33891,7 @@
     </row>
     <row r="298" spans="1:6">
       <c r="A298" s="83"/>
-      <c r="B298" s="200" t="s">
+      <c r="B298" s="202" t="s">
         <v>5865</v>
       </c>
       <c r="C298" t="s">
@@ -33893,7 +33903,7 @@
     </row>
     <row r="299" spans="1:6">
       <c r="A299" s="83"/>
-      <c r="B299" s="200" t="s">
+      <c r="B299" s="202" t="s">
         <v>4387</v>
       </c>
       <c r="C299" t="s">
@@ -33905,7 +33915,7 @@
     </row>
     <row r="300" spans="1:6">
       <c r="A300" s="83"/>
-      <c r="B300" s="200" t="s">
+      <c r="B300" s="202" t="s">
         <v>4806</v>
       </c>
       <c r="C300" t="s">
@@ -33917,7 +33927,7 @@
     </row>
     <row r="301" spans="1:6">
       <c r="A301" s="83"/>
-      <c r="B301" s="200" t="s">
+      <c r="B301" s="202" t="s">
         <v>1216</v>
       </c>
       <c r="C301" t="s">
@@ -33929,7 +33939,7 @@
     </row>
     <row r="302" spans="1:6">
       <c r="A302" s="83"/>
-      <c r="B302" s="200">
+      <c r="B302" s="202">
         <v>13675</v>
       </c>
       <c r="C302" t="s">
@@ -33943,7 +33953,7 @@
     </row>
     <row r="303" spans="1:6">
       <c r="A303" s="83"/>
-      <c r="B303" s="200" t="s">
+      <c r="B303" s="202" t="s">
         <v>830</v>
       </c>
       <c r="C303" t="s">
@@ -33957,7 +33967,7 @@
     </row>
     <row r="304" spans="1:6">
       <c r="A304" s="83"/>
-      <c r="B304" s="200">
+      <c r="B304" s="202">
         <v>98991</v>
       </c>
       <c r="C304" t="s">
@@ -34210,7 +34220,7 @@
     <hyperlink ref="D274" r:id="rId122" xr:uid="{1CB8F24B-B796-4CF1-811C-B93EFC023B79}"/>
     <hyperlink ref="D290" r:id="rId123" xr:uid="{EC6565C7-D170-4D9D-9D08-F4C489F93BBB}"/>
     <hyperlink ref="D295" r:id="rId124" xr:uid="{66F73DCC-AC4E-49E4-B66E-A1F6AA3EDE3D}"/>
-    <hyperlink ref="D26" r:id="rId125" xr:uid="{A9806DFA-0599-4BE2-AE6F-E091049A7AB5}"/>
+    <hyperlink ref="D26" r:id="rId125" xr:uid="{A66E0BEE-2AF9-4A99-9466-415564EA9FC4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId126"/>

</xml_diff>

<commit_message>
Add Contract update / PO Email continuation
</commit_message>
<xml_diff>
--- a/CageCodelist.xlsx
+++ b/CageCodelist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avinash Patel\Desktop\WestSim_App\WestSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A0FE10-15D8-4C60-A585-FA756F411D41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5828A864-9F1A-4510-BA95-863FB94A291C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="16" activeTab="16" xr2:uid="{BFAE7096-C865-48E4-884B-BB11FAFA2759}"/>
   </bookViews>
@@ -1432,7 +1432,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9564" uniqueCount="5968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9596" uniqueCount="5995">
   <si>
     <t>TSE</t>
   </si>
@@ -19418,6 +19418,87 @@
   </si>
   <si>
     <t>Attention: Tony Davis</t>
+  </si>
+  <si>
+    <t>Hiab USA, Inc.</t>
+  </si>
+  <si>
+    <t>702 Columbia Drive</t>
+  </si>
+  <si>
+    <t>Plainfield, IN 46168</t>
+  </si>
+  <si>
+    <t>Phone: 1-800-837-2351</t>
+  </si>
+  <si>
+    <t>ITT Cannon</t>
+  </si>
+  <si>
+    <t>56 Technology Dr.</t>
+  </si>
+  <si>
+    <t>Irvine, CA 92618</t>
+  </si>
+  <si>
+    <t>Attention: Lorraine Cerulli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">425 Hanley Industrial Court </t>
+  </si>
+  <si>
+    <t>St. Louis, MO 63144</t>
+  </si>
+  <si>
+    <t>Phone: 800-243-8162</t>
+  </si>
+  <si>
+    <t>Kooltronic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Pennington-Hopewell Road </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pennington, NJ 08534 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone: (609) 466-3400 </t>
+  </si>
+  <si>
+    <t>KTSDI LLC</t>
+  </si>
+  <si>
+    <t>801 E. Middletown Road</t>
+  </si>
+  <si>
+    <t>North Lima/ YNG, OH 44452</t>
+  </si>
+  <si>
+    <t>Phone: 330-783-2000</t>
+  </si>
+  <si>
+    <t>Leddynamics, Inc.</t>
+  </si>
+  <si>
+    <t>44 Hull ST PO BOX 444 Suite 100</t>
+  </si>
+  <si>
+    <t>Randolph, VT 05060</t>
+  </si>
+  <si>
+    <t>Attention: Bob Sparadeo</t>
+  </si>
+  <si>
+    <t>Mafo Naval Closures BV</t>
+  </si>
+  <si>
+    <t>P.O. Box 212, 7556 AE Almelo</t>
+  </si>
+  <si>
+    <t>the Netherlands</t>
+  </si>
+  <si>
+    <t>Att: Renée de Lange</t>
   </si>
 </sst>
 </file>
@@ -30293,8 +30374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA825E1-D4F3-4B14-9B07-A99A0DC7EB36}">
   <dimension ref="A1:J334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30304,9 +30385,9 @@
     <col min="4" max="4" width="53.42578125" customWidth="1"/>
     <col min="5" max="5" width="37.7109375" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -30825,7 +30906,18 @@
       <c r="E22" s="186" t="s">
         <v>4268</v>
       </c>
-      <c r="F22" s="83"/>
+      <c r="F22" s="83" t="s">
+        <v>5968</v>
+      </c>
+      <c r="G22" s="206" t="s">
+        <v>5969</v>
+      </c>
+      <c r="H22" s="206" t="s">
+        <v>5970</v>
+      </c>
+      <c r="I22" s="206" t="s">
+        <v>5971</v>
+      </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="199"/>
@@ -30839,7 +30931,18 @@
         <v>4267</v>
       </c>
       <c r="E23" s="186"/>
-      <c r="F23" s="83"/>
+      <c r="F23" s="83" t="s">
+        <v>5968</v>
+      </c>
+      <c r="G23" s="206" t="s">
+        <v>5969</v>
+      </c>
+      <c r="H23" s="206" t="s">
+        <v>5970</v>
+      </c>
+      <c r="I23" s="206" t="s">
+        <v>5971</v>
+      </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="199" t="s">
@@ -30855,7 +30958,18 @@
         <v>678</v>
       </c>
       <c r="E24" s="197"/>
-      <c r="F24" s="83"/>
+      <c r="F24" s="83" t="s">
+        <v>5972</v>
+      </c>
+      <c r="G24" s="206" t="s">
+        <v>5973</v>
+      </c>
+      <c r="H24" s="206" t="s">
+        <v>5974</v>
+      </c>
+      <c r="J24" s="207" t="s">
+        <v>5975</v>
+      </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="199"/>
@@ -30869,7 +30983,18 @@
         <v>4322</v>
       </c>
       <c r="E25" s="186"/>
-      <c r="F25" s="83"/>
+      <c r="F25" s="83" t="s">
+        <v>3318</v>
+      </c>
+      <c r="G25" s="206" t="s">
+        <v>5976</v>
+      </c>
+      <c r="H25" s="206" t="s">
+        <v>5977</v>
+      </c>
+      <c r="I25" s="206" t="s">
+        <v>5978</v>
+      </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="199"/>
@@ -30909,7 +31034,7 @@
       <c r="E28" s="186"/>
       <c r="F28" s="83"/>
     </row>
-    <row r="29" spans="1:10" ht="19.899999999999999" customHeight="1">
+    <row r="29" spans="1:10">
       <c r="A29" s="199"/>
       <c r="B29" s="201" t="s">
         <v>987</v>
@@ -30921,9 +31046,20 @@
         <v>5857</v>
       </c>
       <c r="E29" s="186"/>
-      <c r="F29" s="83"/>
-    </row>
-    <row r="30" spans="1:10" ht="16.5" customHeight="1">
+      <c r="F29" s="83" t="s">
+        <v>5979</v>
+      </c>
+      <c r="G29" s="206" t="s">
+        <v>5980</v>
+      </c>
+      <c r="H29" s="206" t="s">
+        <v>5981</v>
+      </c>
+      <c r="I29" s="206" t="s">
+        <v>5982</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="199"/>
       <c r="B30" s="200" t="s">
         <v>1673</v>
@@ -30935,7 +31071,18 @@
         <v>1674</v>
       </c>
       <c r="E30" s="186"/>
-      <c r="F30" s="83"/>
+      <c r="F30" s="83" t="s">
+        <v>5983</v>
+      </c>
+      <c r="G30" s="212" t="s">
+        <v>5984</v>
+      </c>
+      <c r="H30" s="207" t="s">
+        <v>5985</v>
+      </c>
+      <c r="I30" s="207" t="s">
+        <v>5986</v>
+      </c>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1">
       <c r="A31" s="199"/>
@@ -30961,7 +31108,7 @@
       <c r="E32" s="186"/>
       <c r="F32" s="83"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:10">
       <c r="A33" s="199"/>
       <c r="B33" s="200" t="s">
         <v>5881</v>
@@ -30973,7 +31120,7 @@
       <c r="E33" s="186"/>
       <c r="F33" s="83"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:10">
       <c r="A34" s="199"/>
       <c r="B34" s="202" t="s">
         <v>502</v>
@@ -30985,9 +31132,20 @@
         <v>641</v>
       </c>
       <c r="E34" s="186"/>
-      <c r="F34" s="83"/>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="F34" s="83" t="s">
+        <v>5987</v>
+      </c>
+      <c r="G34" s="212" t="s">
+        <v>5988</v>
+      </c>
+      <c r="H34" s="207" t="s">
+        <v>5989</v>
+      </c>
+      <c r="J34" s="207" t="s">
+        <v>5990</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="199"/>
       <c r="B35" s="202" t="s">
         <v>4469</v>
@@ -30999,7 +31157,7 @@
       <c r="E35" s="186"/>
       <c r="F35" s="83"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:10">
       <c r="A36" s="199"/>
       <c r="B36" s="200" t="s">
         <v>1166</v>
@@ -31011,9 +31169,20 @@
         <v>4286</v>
       </c>
       <c r="E36" s="186"/>
-      <c r="F36" s="83"/>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="F36" s="206" t="s">
+        <v>5991</v>
+      </c>
+      <c r="G36" s="206" t="s">
+        <v>5992</v>
+      </c>
+      <c r="H36" s="206" t="s">
+        <v>5993</v>
+      </c>
+      <c r="J36" s="206" t="s">
+        <v>5994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="199"/>
       <c r="B37" s="200">
         <v>87009</v>
@@ -31027,7 +31196,7 @@
       <c r="E37" s="186"/>
       <c r="F37" s="83"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:10">
       <c r="A38" s="199"/>
       <c r="B38" s="200" t="s">
         <v>4441</v>
@@ -31039,7 +31208,7 @@
       <c r="E38" s="186"/>
       <c r="F38" s="83"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:10">
       <c r="A39" s="199" t="s">
         <v>1913</v>
       </c>
@@ -31055,7 +31224,7 @@
       <c r="E39" s="186"/>
       <c r="F39" s="83"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:10">
       <c r="A40" s="199"/>
       <c r="B40" s="200" t="s">
         <v>449</v>
@@ -31069,7 +31238,7 @@
       <c r="E40" s="197"/>
       <c r="F40" s="83"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:10">
       <c r="A41" s="199"/>
       <c r="B41" s="200" t="s">
         <v>985</v>
@@ -31083,7 +31252,7 @@
       <c r="E41" s="186"/>
       <c r="F41" s="83"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:10">
       <c r="A42" s="199"/>
       <c r="B42" s="200" t="s">
         <v>225</v>
@@ -31097,7 +31266,7 @@
       <c r="E42" s="186"/>
       <c r="F42" s="83"/>
     </row>
-    <row r="43" spans="1:6" ht="18" customHeight="1">
+    <row r="43" spans="1:10" ht="18" customHeight="1">
       <c r="A43" s="199"/>
       <c r="B43" s="200">
         <v>32387</v>
@@ -31111,7 +31280,7 @@
       <c r="E43" s="186"/>
       <c r="F43" s="83"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:10">
       <c r="A44" s="199"/>
       <c r="B44" s="200" t="s">
         <v>818</v>
@@ -31125,7 +31294,7 @@
       <c r="E44" s="186"/>
       <c r="F44" s="83"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:10">
       <c r="A45" s="199"/>
       <c r="B45" s="200" t="s">
         <v>456</v>
@@ -31137,7 +31306,7 @@
       <c r="E45" s="186"/>
       <c r="F45" s="83"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:10">
       <c r="A46" s="199"/>
       <c r="B46" s="200" t="s">
         <v>616</v>
@@ -31151,7 +31320,7 @@
       <c r="E46" s="186"/>
       <c r="F46" s="83"/>
     </row>
-    <row r="47" spans="1:6" ht="16.899999999999999" customHeight="1">
+    <row r="47" spans="1:10" ht="16.899999999999999" customHeight="1">
       <c r="A47" s="199"/>
       <c r="B47" s="200" t="s">
         <v>4311</v>
@@ -31165,7 +31334,7 @@
       <c r="E47" s="186"/>
       <c r="F47" s="83"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:10">
       <c r="A48" s="199"/>
       <c r="B48" s="200" t="s">
         <v>4419</v>

</xml_diff>

<commit_message>
PO Creation mostly done, work on connecting to main workbook
</commit_message>
<xml_diff>
--- a/CageCodelist.xlsx
+++ b/CageCodelist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avinash Patel\Desktop\WestSim_App\WestSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDAEDA6-BB38-4124-BEB5-6290EE94EE61}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AF3187-4031-4D49-9C4F-FC5B630953E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1470" windowWidth="29040" windowHeight="15840" firstSheet="16" activeTab="16" xr2:uid="{BFAE7096-C865-48E4-884B-BB11FAFA2759}"/>
   </bookViews>
@@ -1432,7 +1432,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9766" uniqueCount="6153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9767" uniqueCount="6154">
   <si>
     <t>TSE</t>
   </si>
@@ -19973,6 +19973,9 @@
   <si>
     <t>Attention: Deanna Howell</t>
   </si>
+  <si>
+    <t>alphonso.brooks@standardcal.com</t>
+  </si>
 </sst>
 </file>
 
@@ -19984,7 +19987,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
-  <fonts count="65">
+  <fonts count="64">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -20394,15 +20397,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -20425,7 +20419,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -20513,12 +20507,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF0F0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -20759,7 +20747,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="57" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="57" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -20999,7 +20987,7 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="17" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="57" fillId="16" borderId="0" xfId="4"/>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -21015,24 +21003,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="58" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -30858,8 +30846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA825E1-D4F3-4B14-9B07-A99A0DC7EB36}">
   <dimension ref="A1:J305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="F311" sqref="F311"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30980,7 +30968,7 @@
       <c r="C6" t="s">
         <v>172</v>
       </c>
-      <c r="D6" s="186" t="s">
+      <c r="D6" s="10" t="s">
         <v>4242</v>
       </c>
       <c r="E6" s="186"/>
@@ -31026,13 +31014,13 @@
       <c r="D8" s="204" t="s">
         <v>5843</v>
       </c>
-      <c r="E8" s="186" t="s">
+      <c r="E8" s="10" t="s">
         <v>4246</v>
       </c>
       <c r="F8" s="83" t="s">
         <v>5904</v>
       </c>
-      <c r="G8" s="211" t="s">
+      <c r="G8" s="209" t="s">
         <v>5905</v>
       </c>
       <c r="H8" s="206" t="s">
@@ -31083,10 +31071,10 @@
       <c r="F10" s="83" t="s">
         <v>5911</v>
       </c>
-      <c r="G10" s="212" t="s">
+      <c r="G10" s="210" t="s">
         <v>5913</v>
       </c>
-      <c r="H10" s="212" t="s">
+      <c r="H10" s="210" t="s">
         <v>5914</v>
       </c>
       <c r="J10" s="206" t="s">
@@ -31170,7 +31158,7 @@
       <c r="F14" s="83" t="s">
         <v>5929</v>
       </c>
-      <c r="G14" s="211" t="s">
+      <c r="G14" s="209" t="s">
         <v>5930</v>
       </c>
       <c r="H14" s="206" t="s">
@@ -31270,7 +31258,9 @@
         <v>88</v>
       </c>
       <c r="D18" s="186"/>
-      <c r="E18" s="186"/>
+      <c r="E18" s="10" t="s">
+        <v>6153</v>
+      </c>
       <c r="F18" s="83" t="s">
         <v>4854</v>
       </c>
@@ -31332,7 +31322,7 @@
       <c r="F20" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="211" t="s">
+      <c r="G20" s="209" t="s">
         <v>5950</v>
       </c>
       <c r="H20" s="206" t="s">
@@ -31591,7 +31581,7 @@
       <c r="F32" s="83" t="s">
         <v>5973</v>
       </c>
-      <c r="G32" s="211" t="s">
+      <c r="G32" s="209" t="s">
         <v>5974</v>
       </c>
       <c r="H32" s="206" t="s">
@@ -31652,7 +31642,7 @@
       <c r="F36" s="83" t="s">
         <v>5977</v>
       </c>
-      <c r="G36" s="211" t="s">
+      <c r="G36" s="209" t="s">
         <v>5978</v>
       </c>
       <c r="H36" s="206" t="s">
@@ -31738,7 +31728,7 @@
       <c r="F41" s="83" t="s">
         <v>5985</v>
       </c>
-      <c r="G41" s="211" t="s">
+      <c r="G41" s="209" t="s">
         <v>5986</v>
       </c>
       <c r="H41" s="206" t="s">
@@ -31785,7 +31775,7 @@
       <c r="F43" s="83" t="s">
         <v>5992</v>
       </c>
-      <c r="G43" s="211" t="s">
+      <c r="G43" s="209" t="s">
         <v>5993</v>
       </c>
       <c r="H43" s="206" t="s">
@@ -31807,7 +31797,7 @@
         <v>438</v>
       </c>
       <c r="E44" s="186"/>
-      <c r="F44" s="213" t="s">
+      <c r="F44" s="211" t="s">
         <v>5996</v>
       </c>
       <c r="G44" t="s">
@@ -31866,7 +31856,7 @@
       <c r="F46" s="83" t="s">
         <v>6005</v>
       </c>
-      <c r="G46" s="211" t="s">
+      <c r="G46" s="209" t="s">
         <v>6006</v>
       </c>
       <c r="H46" s="206" t="s">
@@ -31900,7 +31890,7 @@
       <c r="F48" s="83" t="s">
         <v>6008</v>
       </c>
-      <c r="G48" s="211" t="s">
+      <c r="G48" s="209" t="s">
         <v>6009</v>
       </c>
       <c r="H48" s="206" t="s">
@@ -31922,7 +31912,7 @@
       <c r="F49" s="83" t="s">
         <v>1958</v>
       </c>
-      <c r="G49" s="211" t="s">
+      <c r="G49" s="209" t="s">
         <v>6011</v>
       </c>
       <c r="H49" s="206" t="s">
@@ -31947,7 +31937,7 @@
       <c r="F50" s="83" t="s">
         <v>4136</v>
       </c>
-      <c r="G50" s="211" t="s">
+      <c r="G50" s="209" t="s">
         <v>6015</v>
       </c>
       <c r="H50" s="206" t="s">
@@ -31994,7 +31984,7 @@
       <c r="F52" s="83" t="s">
         <v>6020</v>
       </c>
-      <c r="G52" s="211" t="s">
+      <c r="G52" s="209" t="s">
         <v>6021</v>
       </c>
       <c r="H52" s="206" t="s">
@@ -32075,7 +32065,7 @@
       <c r="F56" s="83" t="s">
         <v>6033</v>
       </c>
-      <c r="G56" s="211" t="s">
+      <c r="G56" s="209" t="s">
         <v>6034</v>
       </c>
       <c r="H56" s="206" t="s">
@@ -32100,10 +32090,10 @@
       <c r="F57" s="83" t="s">
         <v>2429</v>
       </c>
-      <c r="G57" s="212" t="s">
+      <c r="G57" s="210" t="s">
         <v>6037</v>
       </c>
-      <c r="H57" s="212" t="s">
+      <c r="H57" s="210" t="s">
         <v>6038</v>
       </c>
       <c r="I57" s="206" t="s">
@@ -32155,7 +32145,7 @@
         <v>520</v>
       </c>
       <c r="D61" s="186"/>
-      <c r="E61" s="207"/>
+      <c r="E61" s="213"/>
       <c r="F61" s="83"/>
     </row>
     <row r="62" spans="1:10">
@@ -32170,7 +32160,7 @@
         <v>670</v>
       </c>
       <c r="E62" s="186"/>
-      <c r="F62" s="209"/>
+      <c r="F62" s="214"/>
     </row>
     <row r="63" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="A63" s="199"/>
@@ -32197,7 +32187,7 @@
       <c r="D64" s="10" t="s">
         <v>5815</v>
       </c>
-      <c r="E64" s="208"/>
+      <c r="E64" s="207"/>
       <c r="F64" s="83"/>
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1">
@@ -32212,7 +32202,7 @@
         <v>4294</v>
       </c>
       <c r="E65" s="186"/>
-      <c r="F65" s="210"/>
+      <c r="F65" s="208"/>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="199"/>
@@ -32229,7 +32219,7 @@
       <c r="F66" s="83" t="s">
         <v>6040</v>
       </c>
-      <c r="G66" s="214" t="s">
+      <c r="G66" s="212" t="s">
         <v>6041</v>
       </c>
       <c r="H66" s="206" t="s">
@@ -32330,7 +32320,7 @@
       <c r="F71" s="83" t="s">
         <v>6052</v>
       </c>
-      <c r="G71" s="211" t="s">
+      <c r="G71" s="209" t="s">
         <v>6053</v>
       </c>
       <c r="H71" s="206" t="s">
@@ -32399,7 +32389,7 @@
       <c r="F75" s="83" t="s">
         <v>6056</v>
       </c>
-      <c r="G75" s="211" t="s">
+      <c r="G75" s="209" t="s">
         <v>6057</v>
       </c>
       <c r="H75" s="206" t="s">
@@ -32452,7 +32442,7 @@
       <c r="F77" s="83" t="s">
         <v>6066</v>
       </c>
-      <c r="G77" s="211" t="s">
+      <c r="G77" s="209" t="s">
         <v>6067</v>
       </c>
       <c r="H77" s="206" t="s">
@@ -32933,7 +32923,7 @@
       <c r="F112" s="83" t="s">
         <v>6078</v>
       </c>
-      <c r="G112" s="211" t="s">
+      <c r="G112" s="209" t="s">
         <v>6079</v>
       </c>
       <c r="H112" s="206" t="s">
@@ -33163,7 +33153,7 @@
       <c r="F126" s="83" t="s">
         <v>6097</v>
       </c>
-      <c r="G126" s="211" t="s">
+      <c r="G126" s="209" t="s">
         <v>6098</v>
       </c>
       <c r="H126" s="206" t="s">
@@ -33290,7 +33280,7 @@
       <c r="F135" s="83" t="s">
         <v>6101</v>
       </c>
-      <c r="G135" s="211" t="s">
+      <c r="G135" s="209" t="s">
         <v>6102</v>
       </c>
       <c r="H135" s="206" t="s">
@@ -33541,7 +33531,7 @@
       <c r="F152" s="83" t="s">
         <v>2252</v>
       </c>
-      <c r="G152" s="211" t="s">
+      <c r="G152" s="209" t="s">
         <v>6115</v>
       </c>
       <c r="H152" s="206" t="s">
@@ -33706,7 +33696,7 @@
       <c r="F163" s="83" t="s">
         <v>4780</v>
       </c>
-      <c r="G163" s="211" t="s">
+      <c r="G163" s="209" t="s">
         <v>6123</v>
       </c>
       <c r="H163" s="206" t="s">
@@ -34008,7 +33998,7 @@
       <c r="F186" s="83" t="s">
         <v>6127</v>
       </c>
-      <c r="G186" s="211" t="s">
+      <c r="G186" s="209" t="s">
         <v>6128</v>
       </c>
       <c r="H186" s="206" t="s">
@@ -35360,10 +35350,10 @@
         <v>5864</v>
       </c>
       <c r="E291" s="186"/>
-      <c r="F291" s="211" t="s">
+      <c r="F291" s="209" t="s">
         <v>6144</v>
       </c>
-      <c r="G291" s="211" t="s">
+      <c r="G291" s="209" t="s">
         <v>6145</v>
       </c>
       <c r="H291" s="206" t="s">
@@ -35539,7 +35529,7 @@
       <c r="F304" s="83" t="s">
         <v>6149</v>
       </c>
-      <c r="G304" s="211" t="s">
+      <c r="G304" s="209" t="s">
         <v>6150</v>
       </c>
       <c r="H304" s="206" t="s">
@@ -35687,9 +35677,10 @@
     <hyperlink ref="D102" r:id="rId118" xr:uid="{53041BB8-8F5E-429C-BA8B-AC0D21FB3C9A}"/>
     <hyperlink ref="D26" r:id="rId119" xr:uid="{52023773-05B7-476D-B81A-C12EBF8E9E51}"/>
     <hyperlink ref="E72" r:id="rId120" xr:uid="{5C2D91B8-9071-4EC7-9598-883D8C911AF4}"/>
+    <hyperlink ref="E18" r:id="rId121" xr:uid="{E566AF6D-1CB5-4948-B035-53C2C907D480}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId121"/>
+  <pageSetup orientation="portrait" r:id="rId122"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add Contract bug fix / cage code list update
</commit_message>
<xml_diff>
--- a/CageCodelist.xlsx
+++ b/CageCodelist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avinash Patel\Desktop\WestSim_App\WestSim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Kalwar\Documents\WestSim_Shared\WestSim\AADASHBOARD\FEB19\Cagecodelist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CB5A07-E5C0-45DA-8D45-648C75D19A6D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C030785-44E7-46E3-8FDC-8D9BB9198863}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="16" activeTab="16" xr2:uid="{BFAE7096-C865-48E4-884B-BB11FAFA2759}"/>
+    <workbookView xWindow="30" yWindow="630" windowWidth="20460" windowHeight="10890" firstSheet="16" activeTab="16" xr2:uid="{BFAE7096-C865-48E4-884B-BB11FAFA2759}"/>
   </bookViews>
   <sheets>
     <sheet name="QuoteCal" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1432,7 +1432,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9896" uniqueCount="6161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9886" uniqueCount="6160">
   <si>
     <t>TSE</t>
   </si>
@@ -19989,13 +19989,10 @@
     <t>angelinaherrera@moldeddevices.com</t>
   </si>
   <si>
+    <t>kathyj@philagear.com ; gquinlan@philagear.com</t>
+  </si>
+  <si>
     <t>thysee@theleeco.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kathyj@philagear.com </t>
-  </si>
-  <si>
-    <t>gquinlan@philagear.com</t>
   </si>
 </sst>
 </file>
@@ -30864,10 +30861,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA825E1-D4F3-4B14-9B07-A99A0DC7EB36}">
-  <dimension ref="A1:K333"/>
+  <dimension ref="A1:J333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30875,7 +30872,7 @@
     <col min="2" max="2" width="7.7109375" customWidth="1"/>
     <col min="3" max="3" width="51.5703125" customWidth="1"/>
     <col min="4" max="4" width="53.42578125" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
@@ -30926,9 +30923,7 @@
       <c r="D2" s="10" t="s">
         <v>6148</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>6148</v>
-      </c>
+      <c r="E2" s="186"/>
       <c r="F2" s="83"/>
     </row>
     <row r="3" spans="1:10">
@@ -30942,9 +30937,7 @@
       <c r="D3" s="10" t="s">
         <v>6149</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>6149</v>
-      </c>
+      <c r="E3" s="83"/>
       <c r="F3" s="83" t="s">
         <v>1999</v>
       </c>
@@ -31159,9 +31152,7 @@
       <c r="D12" s="10" t="s">
         <v>6151</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>6151</v>
-      </c>
+      <c r="E12" s="10"/>
       <c r="F12" s="83" t="s">
         <v>5916</v>
       </c>
@@ -31313,9 +31304,10 @@
       <c r="C18" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>6152</v>
       </c>
+      <c r="E18" s="186"/>
       <c r="F18" s="83" t="s">
         <v>4850</v>
       </c>
@@ -31402,9 +31394,7 @@
       <c r="D21" s="10" t="s">
         <v>6153</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>6153</v>
-      </c>
+      <c r="E21" s="10"/>
       <c r="F21" s="83" t="s">
         <v>5949</v>
       </c>
@@ -31617,9 +31607,7 @@
       <c r="D30" s="10" t="s">
         <v>6154</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>6154</v>
-      </c>
+      <c r="E30" s="186"/>
       <c r="F30" s="83"/>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1">
@@ -31750,9 +31738,7 @@
       <c r="D37" s="10" t="s">
         <v>6155</v>
       </c>
-      <c r="E37" s="10" t="s">
-        <v>6155</v>
-      </c>
+      <c r="E37" s="186"/>
       <c r="F37" s="83"/>
     </row>
     <row r="38" spans="1:10">
@@ -31766,9 +31752,7 @@
       <c r="D38" s="10" t="s">
         <v>6156</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>6156</v>
-      </c>
+      <c r="E38" s="10"/>
       <c r="F38" s="204" t="s">
         <v>5977</v>
       </c>
@@ -31819,9 +31803,7 @@
       <c r="D41" s="10" t="s">
         <v>6157</v>
       </c>
-      <c r="E41" s="10" t="s">
-        <v>6157</v>
-      </c>
+      <c r="E41" s="10"/>
       <c r="F41" s="83" t="s">
         <v>5981</v>
       </c>
@@ -32323,7 +32305,7 @@
       </c>
       <c r="F64" s="83"/>
     </row>
-    <row r="65" spans="1:11" ht="15.75" thickBot="1">
+    <row r="65" spans="1:10" ht="15.75" thickBot="1">
       <c r="A65" s="198"/>
       <c r="B65" s="199">
         <v>24602</v>
@@ -32339,7 +32321,7 @@
       </c>
       <c r="F65" s="207"/>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:10">
       <c r="A66" s="198"/>
       <c r="B66" s="199" t="s">
         <v>4329</v>
@@ -32366,7 +32348,7 @@
         <v>5896</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:10">
       <c r="A67" s="198"/>
       <c r="B67" s="199" t="s">
         <v>4359</v>
@@ -32382,7 +32364,7 @@
       </c>
       <c r="F67" s="83"/>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:10">
       <c r="A68" s="198"/>
       <c r="B68" s="199">
         <v>64411</v>
@@ -32398,7 +32380,7 @@
       </c>
       <c r="F68" s="83"/>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:10">
       <c r="A69" s="198"/>
       <c r="B69" s="199" t="s">
         <v>376</v>
@@ -32421,7 +32403,7 @@
         <v>6046</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:10">
       <c r="A70" s="198"/>
       <c r="B70" s="199" t="s">
         <v>5826</v>
@@ -32429,12 +32411,10 @@
       <c r="C70" t="s">
         <v>508</v>
       </c>
-      <c r="D70" s="10" t="s">
-        <v>6159</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>6159</v>
-      </c>
+      <c r="D70" s="186" t="s">
+        <v>6158</v>
+      </c>
+      <c r="E70" s="186"/>
       <c r="F70" s="83" t="s">
         <v>6039</v>
       </c>
@@ -32447,11 +32427,8 @@
       <c r="J70" s="205" t="s">
         <v>6042</v>
       </c>
-      <c r="K70" s="10" t="s">
-        <v>6160</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11">
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="198"/>
       <c r="B71" s="199" t="s">
         <v>4406</v>
@@ -32478,7 +32455,7 @@
         <v>6050</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15" customHeight="1">
+    <row r="72" spans="1:10" ht="15" customHeight="1">
       <c r="A72" s="198"/>
       <c r="B72" s="199" t="s">
         <v>4436</v>
@@ -32494,7 +32471,7 @@
       </c>
       <c r="F72" s="83"/>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:10">
       <c r="A73" s="198"/>
       <c r="B73" s="199" t="s">
         <v>1632</v>
@@ -32510,7 +32487,7 @@
       </c>
       <c r="F73" s="83"/>
     </row>
-    <row r="74" spans="1:11" ht="17.649999999999999" customHeight="1">
+    <row r="74" spans="1:10" ht="17.649999999999999" customHeight="1">
       <c r="A74" s="198"/>
       <c r="B74" s="199">
         <v>44256</v>
@@ -32526,7 +32503,7 @@
       </c>
       <c r="F74" s="83"/>
     </row>
-    <row r="75" spans="1:11" ht="16.149999999999999" customHeight="1">
+    <row r="75" spans="1:10" ht="16.149999999999999" customHeight="1">
       <c r="A75" s="198"/>
       <c r="B75" s="199" t="s">
         <v>1573</v>
@@ -32556,7 +32533,7 @@
         <v>6055</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:10">
       <c r="A76" s="198"/>
       <c r="B76" s="199" t="s">
         <v>4362</v>
@@ -32583,7 +32560,7 @@
         <v>6060</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:10">
       <c r="A77" s="198"/>
       <c r="B77" s="199" t="s">
         <v>4749</v>
@@ -32613,7 +32590,7 @@
         <v>6065</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:10">
       <c r="A78" s="198"/>
       <c r="B78" s="199" t="s">
         <v>1168</v>
@@ -32629,7 +32606,7 @@
       </c>
       <c r="F78" s="83"/>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:10">
       <c r="A79" s="83"/>
       <c r="B79" s="199" t="s">
         <v>4456</v>
@@ -32641,7 +32618,7 @@
       <c r="E79" s="186"/>
       <c r="F79" s="83"/>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:10">
       <c r="A80" s="83"/>
       <c r="B80" s="199" t="s">
         <v>5829</v>
@@ -34397,7 +34374,7 @@
         <v>169</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>6158</v>
+        <v>6159</v>
       </c>
       <c r="E198" s="186"/>
       <c r="F198" s="83"/>
@@ -36179,26 +36156,15 @@
     <hyperlink ref="D3" r:id="rId233" xr:uid="{E1F4BD84-941A-41AF-B77C-39523E08042C}"/>
     <hyperlink ref="D9" r:id="rId234" xr:uid="{CBAE0DF8-B002-429C-9AEB-FD9E61EE9362}"/>
     <hyperlink ref="D12" r:id="rId235" xr:uid="{41A46595-BF21-49EE-AFE5-187231C65658}"/>
-    <hyperlink ref="E18" r:id="rId236" xr:uid="{25B6EDCF-28BE-4C0A-85AA-EDC1BAB31E4E}"/>
+    <hyperlink ref="D18" r:id="rId236" xr:uid="{25B6EDCF-28BE-4C0A-85AA-EDC1BAB31E4E}"/>
     <hyperlink ref="D21" r:id="rId237" xr:uid="{F1DDAE33-7BD9-40EE-9508-E6DDCC4B7B25}"/>
     <hyperlink ref="D30" r:id="rId238" xr:uid="{D8C4CBE7-FC7A-4B13-A1BD-5383C1C0EDBD}"/>
     <hyperlink ref="D37" r:id="rId239" xr:uid="{C4B34480-B00A-43DF-851A-2EC45E7F4637}"/>
     <hyperlink ref="D38" r:id="rId240" xr:uid="{CD02149C-DA19-4D37-8D7C-854D15934153}"/>
     <hyperlink ref="D198" r:id="rId241" xr:uid="{6BA35E2A-1058-4829-86C3-37A0D4FA06C2}"/>
-    <hyperlink ref="E2" r:id="rId242" xr:uid="{4E77B4D0-FBB4-4A36-85A0-F3B897250B7F}"/>
-    <hyperlink ref="E3" r:id="rId243" xr:uid="{A8BBB552-1EDB-4A73-A385-8FD4A49CBB9E}"/>
-    <hyperlink ref="E12" r:id="rId244" xr:uid="{C1A5AD5B-4F52-405F-8F2D-09816F1F3AD7}"/>
-    <hyperlink ref="E21" r:id="rId245" xr:uid="{30B2AF63-21BF-4FE8-B037-57B4B06CFAA1}"/>
-    <hyperlink ref="E30" r:id="rId246" xr:uid="{ED041997-CE3F-401F-ACDE-3B94E32B8B2A}"/>
-    <hyperlink ref="E37" r:id="rId247" xr:uid="{79E67223-3966-41CF-AAAA-4220D0FFF238}"/>
-    <hyperlink ref="E38" r:id="rId248" xr:uid="{188685DE-CF03-4287-83AC-70210C82010C}"/>
-    <hyperlink ref="E41" r:id="rId249" xr:uid="{7D9E69EB-278E-4FA2-B669-82D6222CEA36}"/>
-    <hyperlink ref="D70" r:id="rId250" xr:uid="{6EDBE4DC-7524-4B11-9309-2A10C831CF55}"/>
-    <hyperlink ref="K70" r:id="rId251" xr:uid="{E8667CDA-26CD-4759-8D52-4F1578D75E22}"/>
-    <hyperlink ref="E70" r:id="rId252" xr:uid="{36C3E570-0C9F-4600-8611-CC66BF9435F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId253"/>
+  <pageSetup orientation="portrait" r:id="rId242"/>
 </worksheet>
 </file>
 

</xml_diff>